<commit_message>
Complate on MGL Summary Report
</commit_message>
<xml_diff>
--- a/src/main/resources/template/MGL-Summary.xlsx
+++ b/src/main/resources/template/MGL-Summary.xlsx
@@ -2,18 +2,19 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="330" windowWidth="18915" windowHeight="11145" tabRatio="913" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="330" windowWidth="18915" windowHeight="11145" tabRatio="913" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="MGL Summary" sheetId="4" r:id="rId1"/>
     <sheet name="MGL By Campaign" sheetId="6" r:id="rId2"/>
     <sheet name="MGL By Campaign Total" sheetId="8" r:id="rId3"/>
     <sheet name="Plan LV Template" sheetId="5" r:id="rId4"/>
+    <sheet name="Campaign Name for MGL" sheetId="9" r:id="rId5"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId5"/>
+    <externalReference r:id="rId6"/>
   </externalReferences>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'MGL Summary'!$A$5:$K$13</definedName>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="105">
   <si>
     <t>App(s)</t>
   </si>
@@ -264,6 +265,84 @@
   </si>
   <si>
     <t>No. of Yes file</t>
+  </si>
+  <si>
+    <t>MTI Kbank DDOP Safety Care</t>
+  </si>
+  <si>
+    <t>021DP1715M01</t>
+  </si>
+  <si>
+    <t>MTI Kbank DDOP PA Cash Back</t>
+  </si>
+  <si>
+    <t>021DP1715M02</t>
+  </si>
+  <si>
+    <t>MTI Kbank DDOP POM PA Cash Back</t>
+  </si>
+  <si>
+    <t>021PA1715M03</t>
+  </si>
+  <si>
+    <t>MTLife Kbank DDOP HIP</t>
+  </si>
+  <si>
+    <t>021DP1715L01</t>
+  </si>
+  <si>
+    <t>MTLife Kbank POM Cash Back</t>
+  </si>
+  <si>
+    <t>021PA1715L02</t>
+  </si>
+  <si>
+    <t>MTLife Kbank Health Return Cash</t>
+  </si>
+  <si>
+    <t>021DP1715L03</t>
+  </si>
+  <si>
+    <t>MSIG UOB Super Care</t>
+  </si>
+  <si>
+    <t>151CR1715S01</t>
+  </si>
+  <si>
+    <t>MTLife Broker HIP_OTO</t>
+  </si>
+  <si>
+    <t>141BK1715L04</t>
+  </si>
+  <si>
+    <t>MTLife Broker POM PA OTO</t>
+  </si>
+  <si>
+    <t>141PA1715L05</t>
+  </si>
+  <si>
+    <t>MTLife Broker POM WB OTO</t>
+  </si>
+  <si>
+    <t>141PL1715L06</t>
+  </si>
+  <si>
+    <t>MSIG Broker Happy Life_OTO</t>
+  </si>
+  <si>
+    <t>141BK1715S02</t>
+  </si>
+  <si>
+    <t>MSIG Broker POM PA (OTO)</t>
+  </si>
+  <si>
+    <t>141PA1715S03</t>
+  </si>
+  <si>
+    <t>FWD TVD_OTO</t>
+  </si>
+  <si>
+    <t>171SR3715F01</t>
   </si>
 </sst>
 </file>
@@ -982,9 +1061,6 @@
     <xf numFmtId="167" fontId="18" fillId="9" borderId="14" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="167" fontId="18" fillId="9" borderId="15" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
     <xf numFmtId="167" fontId="16" fillId="9" borderId="13" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
@@ -994,9 +1070,6 @@
     <xf numFmtId="167" fontId="16" fillId="9" borderId="14" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="167" fontId="16" fillId="9" borderId="15" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
     <xf numFmtId="168" fontId="16" fillId="10" borderId="13" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
@@ -1036,9 +1109,6 @@
     <xf numFmtId="167" fontId="16" fillId="11" borderId="14" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="167" fontId="16" fillId="11" borderId="15" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
     <xf numFmtId="168" fontId="16" fillId="11" borderId="13" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
@@ -1096,6 +1166,21 @@
     <xf numFmtId="0" fontId="20" fillId="14" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="167" fontId="13" fillId="9" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="14" fillId="9" borderId="14" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="14" fillId="11" borderId="14" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="13" fillId="9" borderId="14" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="16" fillId="2" borderId="14" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1162,33 +1247,9 @@
     <xf numFmtId="167" fontId="13" fillId="9" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="167" fontId="14" fillId="9" borderId="14" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="14" fillId="9" borderId="15" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="14" fillId="11" borderId="14" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="14" fillId="11" borderId="15" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
     <xf numFmtId="167" fontId="15" fillId="9" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="167" fontId="13" fillId="9" borderId="14" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="13" fillId="9" borderId="15" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="16" fillId="2" borderId="14" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="16" fillId="2" borderId="15" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
     <xf numFmtId="167" fontId="18" fillId="9" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
@@ -1211,6 +1272,24 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="14" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="8" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="8" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1643,6 +1722,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A6:N16"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -1675,36 +1755,36 @@
     </row>
     <row r="7" spans="1:14" ht="11.25" thickBot="1"/>
     <row r="8" spans="1:14" ht="12.75" customHeight="1" thickBot="1">
-      <c r="A8" s="120" t="s">
+      <c r="A8" s="122" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="120" t="s">
+      <c r="B8" s="122" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="122" t="s">
+      <c r="C8" s="124" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="123"/>
-      <c r="E8" s="114" t="s">
+      <c r="D8" s="125"/>
+      <c r="E8" s="116" t="s">
         <v>9</v>
       </c>
-      <c r="F8" s="115"/>
-      <c r="H8" s="116" t="s">
+      <c r="F8" s="117"/>
+      <c r="H8" s="118" t="s">
         <v>3</v>
       </c>
-      <c r="I8" s="116" t="s">
+      <c r="I8" s="118" t="s">
         <v>4</v>
       </c>
-      <c r="J8" s="118" t="s">
+      <c r="J8" s="120" t="s">
         <v>8</v>
       </c>
-      <c r="K8" s="108" t="s">
+      <c r="K8" s="110" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="12.75" customHeight="1" thickBot="1">
-      <c r="A9" s="121"/>
-      <c r="B9" s="121"/>
+      <c r="A9" s="123"/>
+      <c r="B9" s="123"/>
       <c r="C9" s="4" t="s">
         <v>0</v>
       </c>
@@ -1717,10 +1797,10 @@
       <c r="F9" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="H9" s="117"/>
-      <c r="I9" s="117"/>
-      <c r="J9" s="119"/>
-      <c r="K9" s="109"/>
+      <c r="H9" s="119"/>
+      <c r="I9" s="119"/>
+      <c r="J9" s="121"/>
+      <c r="K9" s="111"/>
     </row>
     <row r="10" spans="1:14" s="10" customFormat="1" ht="12.75" customHeight="1" thickBot="1">
       <c r="A10" s="8"/>
@@ -1769,16 +1849,16 @@
       </c>
     </row>
     <row r="13" spans="1:14" s="24" customFormat="1" ht="10.5" customHeight="1" thickBot="1">
-      <c r="A13" s="110" t="s">
+      <c r="A13" s="112" t="s">
         <v>2</v>
       </c>
-      <c r="B13" s="111"/>
+      <c r="B13" s="113"/>
       <c r="C13" s="20"/>
       <c r="D13" s="21"/>
       <c r="E13" s="22"/>
       <c r="F13" s="23"/>
-      <c r="H13" s="112"/>
-      <c r="I13" s="113"/>
+      <c r="H13" s="114"/>
+      <c r="I13" s="115"/>
       <c r="J13" s="25"/>
       <c r="K13" s="26"/>
       <c r="M13" s="27"/>
@@ -1815,10 +1895,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AE44"/>
+  <sheetPr codeName="Sheet2"/>
+  <dimension ref="A1:AD14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1826,21 +1907,20 @@
     <col min="1" max="1" width="14.7109375" style="30" customWidth="1"/>
     <col min="2" max="2" width="16.28515625" style="30" customWidth="1"/>
     <col min="3" max="4" width="13.7109375" style="30" customWidth="1"/>
-    <col min="5" max="5" width="9.28515625" style="30" customWidth="1"/>
-    <col min="6" max="6" width="4.42578125" style="30" customWidth="1"/>
-    <col min="7" max="18" width="13.7109375" style="30" customWidth="1"/>
-    <col min="19" max="19" width="19.85546875" style="30" customWidth="1"/>
-    <col min="20" max="24" width="13.7109375" style="30" customWidth="1"/>
-    <col min="25" max="25" width="2.7109375" style="30" customWidth="1"/>
-    <col min="26" max="31" width="13.7109375" style="30" customWidth="1"/>
-    <col min="32" max="16384" width="9.140625" style="30"/>
+    <col min="5" max="5" width="12.140625" style="30" customWidth="1"/>
+    <col min="6" max="17" width="13.7109375" style="30" customWidth="1"/>
+    <col min="18" max="18" width="19.85546875" style="30" customWidth="1"/>
+    <col min="19" max="23" width="13.7109375" style="30" customWidth="1"/>
+    <col min="24" max="24" width="2.7109375" style="30" customWidth="1"/>
+    <col min="25" max="30" width="13.7109375" style="30" customWidth="1"/>
+    <col min="31" max="16384" width="9.140625" style="30"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" ht="21" customHeight="1">
-      <c r="A1" s="125" t="s">
+    <row r="1" spans="1:30" ht="21" customHeight="1">
+      <c r="A1" s="127" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="125"/>
+      <c r="B1" s="127"/>
       <c r="C1" s="29"/>
       <c r="D1" s="29"/>
       <c r="E1" s="29"/>
@@ -1869,9 +1949,8 @@
       <c r="AB1" s="29"/>
       <c r="AC1" s="29"/>
       <c r="AD1" s="29"/>
-      <c r="AE1" s="29"/>
-    </row>
-    <row r="2" spans="1:31" ht="6.95" customHeight="1">
+    </row>
+    <row r="2" spans="1:30" ht="6.95" customHeight="1">
       <c r="A2" s="29"/>
       <c r="B2" s="29"/>
       <c r="C2" s="29"/>
@@ -1902,16 +1981,15 @@
       <c r="AB2" s="29"/>
       <c r="AC2" s="29"/>
       <c r="AD2" s="29"/>
-      <c r="AE2" s="29"/>
-    </row>
-    <row r="3" spans="1:31" ht="21" customHeight="1">
-      <c r="A3" s="126" t="s">
+    </row>
+    <row r="3" spans="1:30" ht="21" customHeight="1">
+      <c r="A3" s="128" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="126"/>
-      <c r="C3" s="126"/>
-      <c r="D3" s="126"/>
-      <c r="E3" s="126"/>
+      <c r="B3" s="128"/>
+      <c r="C3" s="128"/>
+      <c r="D3" s="128"/>
+      <c r="E3" s="128"/>
       <c r="F3" s="29"/>
       <c r="G3" s="29"/>
       <c r="H3" s="29"/>
@@ -1937,28 +2015,27 @@
       <c r="AB3" s="29"/>
       <c r="AC3" s="29"/>
       <c r="AD3" s="29"/>
-      <c r="AE3" s="29"/>
-    </row>
-    <row r="4" spans="1:31" ht="18" customHeight="1">
-      <c r="A4" s="127" t="s">
+    </row>
+    <row r="4" spans="1:30" ht="18" customHeight="1">
+      <c r="A4" s="129" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="127"/>
-      <c r="C4" s="124" t="s">
+      <c r="B4" s="129"/>
+      <c r="C4" s="126" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="124"/>
-      <c r="E4" s="124"/>
-      <c r="F4" s="124"/>
-      <c r="G4" s="124"/>
-      <c r="H4" s="127" t="s">
+      <c r="D4" s="126"/>
+      <c r="E4" s="126"/>
+      <c r="F4" s="126"/>
+      <c r="G4" s="129" t="s">
         <v>16</v>
       </c>
-      <c r="I4" s="127"/>
-      <c r="J4" s="124" t="s">
+      <c r="H4" s="129"/>
+      <c r="I4" s="126" t="s">
         <v>17</v>
       </c>
-      <c r="K4" s="124"/>
+      <c r="J4" s="126"/>
+      <c r="K4" s="29"/>
       <c r="L4" s="29"/>
       <c r="M4" s="29"/>
       <c r="N4" s="29"/>
@@ -1978,28 +2055,27 @@
       <c r="AB4" s="29"/>
       <c r="AC4" s="29"/>
       <c r="AD4" s="29"/>
-      <c r="AE4" s="29"/>
-    </row>
-    <row r="5" spans="1:31" ht="17.100000000000001" customHeight="1">
-      <c r="A5" s="127" t="s">
+    </row>
+    <row r="5" spans="1:30" ht="17.100000000000001" customHeight="1">
+      <c r="A5" s="129" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="127"/>
-      <c r="C5" s="124" t="s">
+      <c r="B5" s="129"/>
+      <c r="C5" s="126" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="124"/>
-      <c r="E5" s="124"/>
-      <c r="F5" s="124"/>
-      <c r="G5" s="124"/>
-      <c r="H5" s="127" t="s">
+      <c r="D5" s="126"/>
+      <c r="E5" s="126"/>
+      <c r="F5" s="126"/>
+      <c r="G5" s="129" t="s">
         <v>20</v>
       </c>
-      <c r="I5" s="127"/>
-      <c r="J5" s="124" t="s">
+      <c r="H5" s="129"/>
+      <c r="I5" s="126" t="s">
         <v>21</v>
       </c>
-      <c r="K5" s="124"/>
+      <c r="J5" s="126"/>
+      <c r="K5" s="29"/>
       <c r="L5" s="29"/>
       <c r="M5" s="29"/>
       <c r="N5" s="29"/>
@@ -2019,28 +2095,29 @@
       <c r="AB5" s="29"/>
       <c r="AC5" s="29"/>
       <c r="AD5" s="29"/>
-      <c r="AE5" s="29"/>
-    </row>
-    <row r="6" spans="1:31" ht="18.95" customHeight="1">
-      <c r="A6" s="127" t="s">
+    </row>
+    <row r="6" spans="1:30" ht="18.95" customHeight="1">
+      <c r="A6" s="129" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="127"/>
-      <c r="C6" s="128">
+      <c r="B6" s="129"/>
+      <c r="C6" s="130">
         <v>34119</v>
       </c>
-      <c r="D6" s="128"/>
-      <c r="E6" s="128"/>
-      <c r="F6" s="128"/>
-      <c r="G6" s="128"/>
-      <c r="H6" s="129" t="s">
-        <v>23</v>
-      </c>
-      <c r="I6" s="129"/>
-      <c r="J6" s="129" t="s">
-        <v>23</v>
-      </c>
-      <c r="K6" s="129"/>
+      <c r="D6" s="130"/>
+      <c r="E6" s="130"/>
+      <c r="F6" s="130"/>
+      <c r="G6" s="131" t="s">
+        <v>23</v>
+      </c>
+      <c r="H6" s="131"/>
+      <c r="I6" s="131" t="s">
+        <v>23</v>
+      </c>
+      <c r="J6" s="131"/>
+      <c r="K6" s="31" t="s">
+        <v>23</v>
+      </c>
       <c r="L6" s="31" t="s">
         <v>23</v>
       </c>
@@ -2098,22 +2175,21 @@
       <c r="AD6" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="AE6" s="31" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:31" ht="18.95" customHeight="1">
-      <c r="A7" s="134" t="s">
+    </row>
+    <row r="7" spans="1:30" ht="18.95" customHeight="1">
+      <c r="A7" s="132" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="134"/>
-      <c r="C7" s="134" t="s">
+      <c r="B7" s="132"/>
+      <c r="C7" s="132" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="134"/>
-      <c r="E7" s="134"/>
-      <c r="F7" s="134"/>
-      <c r="G7" s="134"/>
+      <c r="D7" s="132"/>
+      <c r="E7" s="132"/>
+      <c r="F7" s="132"/>
+      <c r="G7" s="31" t="s">
+        <v>23</v>
+      </c>
       <c r="H7" s="31" t="s">
         <v>23</v>
       </c>
@@ -2183,11 +2259,8 @@
       <c r="AD7" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="AE7" s="31" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:31" ht="9.9499999999999993" customHeight="1">
+    </row>
+    <row r="8" spans="1:30" ht="9.9499999999999993" customHeight="1">
       <c r="A8" s="31" t="s">
         <v>23</v>
       </c>
@@ -2200,10 +2273,12 @@
       <c r="D8" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="E8" s="129" t="s">
-        <v>23</v>
-      </c>
-      <c r="F8" s="129"/>
+      <c r="E8" s="105" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" s="31" t="s">
+        <v>23</v>
+      </c>
       <c r="G8" s="31" t="s">
         <v>23</v>
       </c>
@@ -2276,11 +2351,8 @@
       <c r="AD8" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="AE8" s="31" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:31" ht="21.95" customHeight="1">
+    </row>
+    <row r="9" spans="1:30" ht="21.95" customHeight="1">
       <c r="A9" s="32" t="s">
         <v>26</v>
       </c>
@@ -2293,87 +2365,86 @@
       <c r="D9" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="E9" s="135" t="s">
+      <c r="E9" s="108" t="s">
         <v>30</v>
       </c>
-      <c r="F9" s="136"/>
+      <c r="F9" s="33" t="s">
+        <v>31</v>
+      </c>
       <c r="G9" s="33" t="s">
-        <v>31</v>
-      </c>
-      <c r="H9" s="33" t="s">
         <v>32</v>
       </c>
+      <c r="H9" s="32" t="s">
+        <v>33</v>
+      </c>
       <c r="I9" s="32" t="s">
-        <v>33</v>
-      </c>
-      <c r="J9" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="K9" s="33" t="s">
+      <c r="J9" s="33" t="s">
         <v>35</v>
       </c>
+      <c r="K9" s="32" t="s">
+        <v>36</v>
+      </c>
       <c r="L9" s="32" t="s">
-        <v>36</v>
-      </c>
-      <c r="M9" s="32" t="s">
         <v>37</v>
       </c>
-      <c r="N9" s="33" t="s">
+      <c r="M9" s="33" t="s">
         <v>38</v>
       </c>
+      <c r="N9" s="32" t="s">
+        <v>39</v>
+      </c>
       <c r="O9" s="32" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="P9" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q9" s="32" t="s">
         <v>41</v>
       </c>
+      <c r="Q9" s="33" t="s">
+        <v>42</v>
+      </c>
       <c r="R9" s="33" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="S9" s="33" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="T9" s="33" t="s">
-        <v>44</v>
-      </c>
-      <c r="U9" s="33" t="s">
         <v>45</v>
       </c>
+      <c r="U9" s="32" t="s">
+        <v>46</v>
+      </c>
       <c r="V9" s="32" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="W9" s="32" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="X9" s="32" t="s">
-        <v>48</v>
-      </c>
-      <c r="Y9" s="32" t="s">
-        <v>23</v>
+        <v>23</v>
+      </c>
+      <c r="Y9" s="33" t="s">
+        <v>49</v>
       </c>
       <c r="Z9" s="33" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="AA9" s="33" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="AB9" s="33" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="AC9" s="33" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="AD9" s="33" t="s">
-        <v>52</v>
-      </c>
-      <c r="AE9" s="33" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="10" spans="1:31" ht="15.95" customHeight="1">
+    <row r="10" spans="1:30" ht="15.95" customHeight="1">
       <c r="A10" s="34" t="s">
         <v>54</v>
       </c>
@@ -2386,87 +2457,86 @@
       <c r="D10" s="35">
         <v>0</v>
       </c>
-      <c r="E10" s="130" t="s">
+      <c r="E10" s="106" t="s">
         <v>56</v>
       </c>
-      <c r="F10" s="131"/>
+      <c r="F10" s="36">
+        <v>6548</v>
+      </c>
       <c r="G10" s="36">
-        <v>6548</v>
-      </c>
-      <c r="H10" s="36">
         <v>4540</v>
       </c>
+      <c r="H10" s="37">
+        <v>25.206234934324062</v>
+      </c>
       <c r="I10" s="37">
-        <v>25.206234934324062</v>
-      </c>
-      <c r="J10" s="37">
         <v>0.69334147831398896</v>
       </c>
-      <c r="K10" s="36">
+      <c r="J10" s="36">
         <v>860</v>
       </c>
+      <c r="K10" s="37">
+        <v>4.774749348792664</v>
+      </c>
       <c r="L10" s="37">
-        <v>4.774749348792664</v>
-      </c>
-      <c r="M10" s="37">
         <v>0.13133781307269396</v>
       </c>
-      <c r="N10" s="38">
+      <c r="M10" s="38">
         <v>20</v>
       </c>
-      <c r="O10" s="37">
+      <c r="N10" s="37">
         <v>0.11104068253006194</v>
       </c>
-      <c r="P10" s="39">
+      <c r="O10" s="39">
         <v>2.3255813953488372E-2</v>
       </c>
-      <c r="Q10" s="34" t="s">
+      <c r="P10" s="34" t="s">
         <v>57</v>
+      </c>
+      <c r="Q10" s="38" t="s">
+        <v>58</v>
       </c>
       <c r="R10" s="38" t="s">
         <v>58</v>
       </c>
-      <c r="S10" s="38" t="s">
+      <c r="S10" s="35">
+        <v>141468</v>
+      </c>
+      <c r="T10" s="35">
+        <v>11789</v>
+      </c>
+      <c r="U10" s="37">
+        <v>589.45000000000005</v>
+      </c>
+      <c r="V10" s="37">
+        <v>7073.4</v>
+      </c>
+      <c r="W10" s="37">
+        <v>54034.25</v>
+      </c>
+      <c r="X10" s="40" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y10" s="38">
+        <v>20</v>
+      </c>
+      <c r="Z10" s="41">
+        <v>2.3255813953488372E-2</v>
+      </c>
+      <c r="AA10" s="42">
+        <v>11789</v>
+      </c>
+      <c r="AB10" s="42">
+        <v>589.45000000000005</v>
+      </c>
+      <c r="AC10" s="38" t="s">
         <v>58</v>
       </c>
-      <c r="T10" s="35">
-        <v>141468</v>
-      </c>
-      <c r="U10" s="35">
-        <v>11789</v>
-      </c>
-      <c r="V10" s="37">
-        <v>589.45000000000005</v>
-      </c>
-      <c r="W10" s="37">
-        <v>7073.4</v>
-      </c>
-      <c r="X10" s="37">
-        <v>54034.25</v>
-      </c>
-      <c r="Y10" s="40" t="s">
-        <v>23</v>
-      </c>
-      <c r="Z10" s="38">
-        <v>20</v>
-      </c>
-      <c r="AA10" s="41">
-        <v>2.3255813953488372E-2</v>
-      </c>
-      <c r="AB10" s="42">
-        <v>11789</v>
-      </c>
-      <c r="AC10" s="42">
-        <v>589.45000000000005</v>
-      </c>
       <c r="AD10" s="38" t="s">
-        <v>58</v>
-      </c>
-      <c r="AE10" s="38" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="11" spans="1:31" ht="15.95" customHeight="1">
+    <row r="11" spans="1:30" ht="15.95" customHeight="1">
       <c r="A11" s="34" t="s">
         <v>59</v>
       </c>
@@ -2479,87 +2549,86 @@
       <c r="D11" s="35">
         <v>427.96666666666664</v>
       </c>
-      <c r="E11" s="130" t="s">
+      <c r="E11" s="106" t="s">
         <v>61</v>
       </c>
-      <c r="F11" s="131"/>
+      <c r="F11" s="36">
+        <v>192</v>
+      </c>
       <c r="G11" s="36">
-        <v>192</v>
-      </c>
-      <c r="H11" s="36">
         <v>83</v>
       </c>
+      <c r="H11" s="37">
+        <v>11.636420281953423</v>
+      </c>
       <c r="I11" s="37">
-        <v>11.636420281953423</v>
-      </c>
-      <c r="J11" s="37">
         <v>0.43229166666666669</v>
       </c>
-      <c r="K11" s="36">
+      <c r="J11" s="36">
         <v>30</v>
       </c>
+      <c r="K11" s="37">
+        <v>4.2059350416699122</v>
+      </c>
       <c r="L11" s="37">
-        <v>4.2059350416699122</v>
-      </c>
-      <c r="M11" s="37">
         <v>0.15625</v>
       </c>
-      <c r="N11" s="38">
+      <c r="M11" s="38">
         <v>20</v>
       </c>
-      <c r="O11" s="37">
+      <c r="N11" s="37">
         <v>2.8039566944466081</v>
       </c>
-      <c r="P11" s="39">
+      <c r="O11" s="39">
         <v>0.66666666666666663</v>
       </c>
-      <c r="Q11" s="34" t="s">
+      <c r="P11" s="34" t="s">
         <v>57</v>
+      </c>
+      <c r="Q11" s="38" t="s">
+        <v>58</v>
       </c>
       <c r="R11" s="38" t="s">
         <v>58</v>
       </c>
-      <c r="S11" s="38" t="s">
+      <c r="S11" s="35">
+        <v>163512</v>
+      </c>
+      <c r="T11" s="35">
+        <v>13626</v>
+      </c>
+      <c r="U11" s="37">
+        <v>681.3</v>
+      </c>
+      <c r="V11" s="37">
+        <v>8175.6</v>
+      </c>
+      <c r="W11" s="37">
+        <v>2139.833333333333</v>
+      </c>
+      <c r="X11" s="40" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y11" s="38">
+        <v>20</v>
+      </c>
+      <c r="Z11" s="41">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="AA11" s="42">
+        <v>13626</v>
+      </c>
+      <c r="AB11" s="42">
+        <v>681.3</v>
+      </c>
+      <c r="AC11" s="38" t="s">
         <v>58</v>
       </c>
-      <c r="T11" s="35">
-        <v>163512</v>
-      </c>
-      <c r="U11" s="35">
-        <v>13626</v>
-      </c>
-      <c r="V11" s="37">
-        <v>681.3</v>
-      </c>
-      <c r="W11" s="37">
-        <v>8175.6</v>
-      </c>
-      <c r="X11" s="37">
-        <v>2139.833333333333</v>
-      </c>
-      <c r="Y11" s="40" t="s">
-        <v>23</v>
-      </c>
-      <c r="Z11" s="38">
-        <v>20</v>
-      </c>
-      <c r="AA11" s="41">
-        <v>0.66666666666666663</v>
-      </c>
-      <c r="AB11" s="42">
-        <v>13626</v>
-      </c>
-      <c r="AC11" s="42">
-        <v>681.3</v>
-      </c>
       <c r="AD11" s="38" t="s">
-        <v>58</v>
-      </c>
-      <c r="AE11" s="38" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="12" spans="1:31" ht="15.95" customHeight="1">
+    <row r="12" spans="1:30" ht="15.95" customHeight="1">
       <c r="A12" s="34" t="s">
         <v>62</v>
       </c>
@@ -2572,87 +2641,86 @@
       <c r="D12" s="35">
         <v>0</v>
       </c>
-      <c r="E12" s="130" t="s">
+      <c r="E12" s="106" t="s">
         <v>64</v>
       </c>
-      <c r="F12" s="131"/>
+      <c r="F12" s="36">
+        <v>22</v>
+      </c>
       <c r="G12" s="36">
-        <v>22</v>
-      </c>
-      <c r="H12" s="36">
         <v>36</v>
       </c>
+      <c r="H12" s="37">
+        <v>0</v>
+      </c>
       <c r="I12" s="37">
-        <v>0</v>
-      </c>
-      <c r="J12" s="37">
         <v>1.6363636363636365</v>
       </c>
-      <c r="K12" s="36">
+      <c r="J12" s="36">
         <v>36</v>
       </c>
+      <c r="K12" s="37">
+        <v>0</v>
+      </c>
       <c r="L12" s="37">
-        <v>0</v>
-      </c>
-      <c r="M12" s="37">
         <v>1.6363636363636365</v>
       </c>
-      <c r="N12" s="38">
+      <c r="M12" s="38">
         <v>8</v>
       </c>
-      <c r="O12" s="37">
-        <v>0</v>
-      </c>
-      <c r="P12" s="39">
+      <c r="N12" s="37">
+        <v>0</v>
+      </c>
+      <c r="O12" s="39">
         <v>0.22222222222222221</v>
       </c>
-      <c r="Q12" s="34" t="s">
+      <c r="P12" s="34" t="s">
         <v>57</v>
+      </c>
+      <c r="Q12" s="38" t="s">
+        <v>58</v>
       </c>
       <c r="R12" s="38" t="s">
         <v>58</v>
       </c>
-      <c r="S12" s="38" t="s">
+      <c r="S12" s="35">
+        <v>63876</v>
+      </c>
+      <c r="T12" s="35">
+        <v>5323</v>
+      </c>
+      <c r="U12" s="37">
+        <v>665.375</v>
+      </c>
+      <c r="V12" s="37">
+        <v>7984.5</v>
+      </c>
+      <c r="W12" s="37">
+        <v>0</v>
+      </c>
+      <c r="X12" s="40" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y12" s="38">
+        <v>8</v>
+      </c>
+      <c r="Z12" s="41">
+        <v>0.22222222222222221</v>
+      </c>
+      <c r="AA12" s="42">
+        <v>5323</v>
+      </c>
+      <c r="AB12" s="42">
+        <v>665.375</v>
+      </c>
+      <c r="AC12" s="38" t="s">
         <v>58</v>
       </c>
-      <c r="T12" s="35">
-        <v>63876</v>
-      </c>
-      <c r="U12" s="35">
-        <v>5323</v>
-      </c>
-      <c r="V12" s="37">
-        <v>665.375</v>
-      </c>
-      <c r="W12" s="37">
-        <v>7984.5</v>
-      </c>
-      <c r="X12" s="37">
-        <v>0</v>
-      </c>
-      <c r="Y12" s="40" t="s">
-        <v>23</v>
-      </c>
-      <c r="Z12" s="38">
-        <v>8</v>
-      </c>
-      <c r="AA12" s="41">
-        <v>0.22222222222222221</v>
-      </c>
-      <c r="AB12" s="42">
-        <v>5323</v>
-      </c>
-      <c r="AC12" s="42">
-        <v>665.375</v>
-      </c>
       <c r="AD12" s="38" t="s">
-        <v>58</v>
-      </c>
-      <c r="AE12" s="38" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="13" spans="1:31" ht="21" customHeight="1">
+    <row r="13" spans="1:30" ht="21" customHeight="1">
       <c r="A13" s="43" t="s">
         <v>65</v>
       </c>
@@ -2665,1192 +2733,163 @@
       <c r="D13" s="44">
         <v>11234.816666666668</v>
       </c>
-      <c r="E13" s="132" t="s">
+      <c r="E13" s="107" t="s">
         <v>66</v>
       </c>
-      <c r="F13" s="133"/>
+      <c r="F13" s="45">
+        <v>6762</v>
+      </c>
       <c r="G13" s="45">
-        <v>6762</v>
-      </c>
-      <c r="H13" s="45">
         <v>4659</v>
       </c>
+      <c r="H13" s="44">
+        <v>24.88158091884009</v>
+      </c>
       <c r="I13" s="44">
-        <v>24.88158091884009</v>
-      </c>
-      <c r="J13" s="44">
         <v>0.6889973380656611</v>
       </c>
-      <c r="K13" s="45">
+      <c r="J13" s="45">
         <v>926</v>
       </c>
+      <c r="K13" s="44">
+        <v>4.945341045470256</v>
+      </c>
       <c r="L13" s="44">
-        <v>4.945341045470256</v>
-      </c>
-      <c r="M13" s="44">
         <v>0.13694173321502515</v>
       </c>
-      <c r="N13" s="43">
+      <c r="M13" s="43">
         <v>48</v>
       </c>
-      <c r="O13" s="44">
+      <c r="N13" s="44">
         <v>0.25634597211940852</v>
       </c>
-      <c r="P13" s="46">
+      <c r="O13" s="46">
         <v>5.183585313174946E-2</v>
       </c>
+      <c r="P13" s="43" t="s">
+        <v>57</v>
+      </c>
       <c r="Q13" s="43" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="R13" s="43" t="s">
         <v>58</v>
       </c>
-      <c r="S13" s="43" t="s">
+      <c r="S13" s="44">
+        <v>368856</v>
+      </c>
+      <c r="T13" s="44">
+        <v>30738</v>
+      </c>
+      <c r="U13" s="44">
+        <v>640.375</v>
+      </c>
+      <c r="V13" s="44">
+        <v>7684.5</v>
+      </c>
+      <c r="W13" s="44">
+        <v>56174.083333333343</v>
+      </c>
+      <c r="X13" s="40" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y13" s="43">
+        <v>48</v>
+      </c>
+      <c r="Z13" s="46">
+        <v>5.183585313174946E-2</v>
+      </c>
+      <c r="AA13" s="47">
+        <v>30738</v>
+      </c>
+      <c r="AB13" s="47">
+        <v>640.375</v>
+      </c>
+      <c r="AC13" s="43" t="s">
         <v>58</v>
       </c>
-      <c r="T13" s="44">
-        <v>368856</v>
-      </c>
-      <c r="U13" s="44">
-        <v>30738</v>
-      </c>
-      <c r="V13" s="44">
-        <v>640.375</v>
-      </c>
-      <c r="W13" s="44">
-        <v>7684.5</v>
-      </c>
-      <c r="X13" s="44">
-        <v>56174.083333333343</v>
-      </c>
-      <c r="Y13" s="40" t="s">
-        <v>23</v>
-      </c>
-      <c r="Z13" s="43">
-        <v>48</v>
-      </c>
-      <c r="AA13" s="46">
-        <v>5.183585313174946E-2</v>
-      </c>
-      <c r="AB13" s="47">
-        <v>30738</v>
-      </c>
-      <c r="AC13" s="47">
-        <v>640.375</v>
-      </c>
       <c r="AD13" s="43" t="s">
-        <v>58</v>
-      </c>
-      <c r="AE13" s="43" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="14" spans="1:31" ht="15.95" hidden="1" customHeight="1">
-      <c r="A14" s="34"/>
-      <c r="B14" s="34"/>
-      <c r="C14" s="35"/>
-      <c r="D14" s="35"/>
-      <c r="E14" s="130"/>
-      <c r="F14" s="131"/>
-      <c r="G14" s="36"/>
-      <c r="H14" s="36"/>
-      <c r="I14" s="37"/>
-      <c r="J14" s="37"/>
-      <c r="K14" s="36"/>
-      <c r="L14" s="37"/>
-      <c r="M14" s="37"/>
-      <c r="N14" s="38"/>
-      <c r="O14" s="37"/>
-      <c r="P14" s="39"/>
-      <c r="Q14" s="34"/>
-      <c r="R14" s="38"/>
-      <c r="S14" s="38"/>
-      <c r="T14" s="35"/>
-      <c r="U14" s="35"/>
-      <c r="V14" s="37"/>
-      <c r="W14" s="37"/>
-      <c r="X14" s="37"/>
-      <c r="Y14" s="40"/>
-      <c r="Z14" s="38"/>
-      <c r="AA14" s="41"/>
-      <c r="AB14" s="42"/>
-      <c r="AC14" s="42"/>
-      <c r="AD14" s="38"/>
-      <c r="AE14" s="38"/>
-    </row>
-    <row r="15" spans="1:31" ht="15.95" hidden="1" customHeight="1">
-      <c r="A15" s="34"/>
-      <c r="B15" s="34"/>
-      <c r="C15" s="35"/>
-      <c r="D15" s="35"/>
-      <c r="E15" s="130"/>
-      <c r="F15" s="131"/>
-      <c r="G15" s="36"/>
-      <c r="H15" s="36"/>
-      <c r="I15" s="37"/>
-      <c r="J15" s="37"/>
-      <c r="K15" s="36"/>
-      <c r="L15" s="37"/>
-      <c r="M15" s="37"/>
-      <c r="N15" s="38"/>
-      <c r="O15" s="37"/>
-      <c r="P15" s="39"/>
-      <c r="Q15" s="34"/>
-      <c r="R15" s="38"/>
-      <c r="S15" s="38"/>
-      <c r="T15" s="35"/>
-      <c r="U15" s="35"/>
-      <c r="V15" s="37"/>
-      <c r="W15" s="37"/>
-      <c r="X15" s="37"/>
-      <c r="Y15" s="40"/>
-      <c r="Z15" s="38"/>
-      <c r="AA15" s="41"/>
-      <c r="AB15" s="42"/>
-      <c r="AC15" s="42"/>
-      <c r="AD15" s="38"/>
-      <c r="AE15" s="38"/>
-    </row>
-    <row r="16" spans="1:31" ht="15.95" hidden="1" customHeight="1">
-      <c r="A16" s="34"/>
-      <c r="B16" s="34"/>
-      <c r="C16" s="35"/>
-      <c r="D16" s="35"/>
-      <c r="E16" s="130"/>
-      <c r="F16" s="131"/>
-      <c r="G16" s="36"/>
-      <c r="H16" s="36"/>
-      <c r="I16" s="37"/>
-      <c r="J16" s="37"/>
-      <c r="K16" s="36"/>
-      <c r="L16" s="37"/>
-      <c r="M16" s="37"/>
-      <c r="N16" s="38"/>
-      <c r="O16" s="37"/>
-      <c r="P16" s="39"/>
-      <c r="Q16" s="34"/>
-      <c r="R16" s="38"/>
-      <c r="S16" s="38"/>
-      <c r="T16" s="35"/>
-      <c r="U16" s="35"/>
-      <c r="V16" s="37"/>
-      <c r="W16" s="37"/>
-      <c r="X16" s="37"/>
-      <c r="Y16" s="40"/>
-      <c r="Z16" s="38"/>
-      <c r="AA16" s="41"/>
-      <c r="AB16" s="42"/>
-      <c r="AC16" s="42"/>
-      <c r="AD16" s="38"/>
-      <c r="AE16" s="38"/>
-    </row>
-    <row r="17" spans="1:31" ht="15.95" hidden="1" customHeight="1">
-      <c r="A17" s="34"/>
-      <c r="B17" s="34"/>
-      <c r="C17" s="35"/>
-      <c r="D17" s="35"/>
-      <c r="E17" s="130"/>
-      <c r="F17" s="131"/>
-      <c r="G17" s="36"/>
-      <c r="H17" s="36"/>
-      <c r="I17" s="37"/>
-      <c r="J17" s="37"/>
-      <c r="K17" s="36"/>
-      <c r="L17" s="37"/>
-      <c r="M17" s="37"/>
-      <c r="N17" s="38"/>
-      <c r="O17" s="37"/>
-      <c r="P17" s="39"/>
-      <c r="Q17" s="34"/>
-      <c r="R17" s="38"/>
-      <c r="S17" s="38"/>
-      <c r="T17" s="35"/>
-      <c r="U17" s="35"/>
-      <c r="V17" s="37"/>
-      <c r="W17" s="37"/>
-      <c r="X17" s="37"/>
-      <c r="Y17" s="40"/>
-      <c r="Z17" s="38"/>
-      <c r="AA17" s="41"/>
-      <c r="AB17" s="42"/>
-      <c r="AC17" s="42"/>
-      <c r="AD17" s="38"/>
-      <c r="AE17" s="38"/>
-    </row>
-    <row r="18" spans="1:31" ht="15.95" hidden="1" customHeight="1">
-      <c r="A18" s="34"/>
-      <c r="B18" s="34"/>
-      <c r="C18" s="35"/>
-      <c r="D18" s="35"/>
-      <c r="E18" s="130"/>
-      <c r="F18" s="131"/>
-      <c r="G18" s="36"/>
-      <c r="H18" s="36"/>
-      <c r="I18" s="37"/>
-      <c r="J18" s="37"/>
-      <c r="K18" s="36"/>
-      <c r="L18" s="37"/>
-      <c r="M18" s="37"/>
-      <c r="N18" s="38"/>
-      <c r="O18" s="37"/>
-      <c r="P18" s="39"/>
-      <c r="Q18" s="34"/>
-      <c r="R18" s="38"/>
-      <c r="S18" s="38"/>
-      <c r="T18" s="35"/>
-      <c r="U18" s="35"/>
-      <c r="V18" s="37"/>
-      <c r="W18" s="37"/>
-      <c r="X18" s="37"/>
-      <c r="Y18" s="40"/>
-      <c r="Z18" s="38"/>
-      <c r="AA18" s="41"/>
-      <c r="AB18" s="42"/>
-      <c r="AC18" s="42"/>
-      <c r="AD18" s="38"/>
-      <c r="AE18" s="38"/>
-    </row>
-    <row r="19" spans="1:31" ht="15.95" hidden="1" customHeight="1">
-      <c r="A19" s="34"/>
-      <c r="B19" s="34"/>
-      <c r="C19" s="35"/>
-      <c r="D19" s="35"/>
-      <c r="E19" s="130"/>
-      <c r="F19" s="131"/>
-      <c r="G19" s="36"/>
-      <c r="H19" s="36"/>
-      <c r="I19" s="37"/>
-      <c r="J19" s="37"/>
-      <c r="K19" s="36"/>
-      <c r="L19" s="37"/>
-      <c r="M19" s="37"/>
-      <c r="N19" s="38"/>
-      <c r="O19" s="37"/>
-      <c r="P19" s="39"/>
-      <c r="Q19" s="34"/>
-      <c r="R19" s="38"/>
-      <c r="S19" s="38"/>
-      <c r="T19" s="35"/>
-      <c r="U19" s="35"/>
-      <c r="V19" s="37"/>
-      <c r="W19" s="37"/>
-      <c r="X19" s="37"/>
-      <c r="Y19" s="40"/>
-      <c r="Z19" s="38"/>
-      <c r="AA19" s="41"/>
-      <c r="AB19" s="42"/>
-      <c r="AC19" s="42"/>
-      <c r="AD19" s="38"/>
-      <c r="AE19" s="38"/>
-    </row>
-    <row r="20" spans="1:31" ht="15.95" hidden="1" customHeight="1">
-      <c r="A20" s="34"/>
-      <c r="B20" s="34"/>
-      <c r="C20" s="35"/>
-      <c r="D20" s="35"/>
-      <c r="E20" s="130"/>
-      <c r="F20" s="131"/>
-      <c r="G20" s="36"/>
-      <c r="H20" s="36"/>
-      <c r="I20" s="37"/>
-      <c r="J20" s="37"/>
-      <c r="K20" s="36"/>
-      <c r="L20" s="37"/>
-      <c r="M20" s="37"/>
-      <c r="N20" s="38"/>
-      <c r="O20" s="37"/>
-      <c r="P20" s="39"/>
-      <c r="Q20" s="34"/>
-      <c r="R20" s="38"/>
-      <c r="S20" s="38"/>
-      <c r="T20" s="35"/>
-      <c r="U20" s="35"/>
-      <c r="V20" s="37"/>
-      <c r="W20" s="37"/>
-      <c r="X20" s="37"/>
-      <c r="Y20" s="40"/>
-      <c r="Z20" s="38"/>
-      <c r="AA20" s="41"/>
-      <c r="AB20" s="42"/>
-      <c r="AC20" s="42"/>
-      <c r="AD20" s="38"/>
-      <c r="AE20" s="38"/>
-    </row>
-    <row r="21" spans="1:31" ht="15.95" hidden="1" customHeight="1">
-      <c r="A21" s="34"/>
-      <c r="B21" s="34"/>
-      <c r="C21" s="35"/>
-      <c r="D21" s="35"/>
-      <c r="E21" s="130"/>
-      <c r="F21" s="131"/>
-      <c r="G21" s="36"/>
-      <c r="H21" s="36"/>
-      <c r="I21" s="37"/>
-      <c r="J21" s="37"/>
-      <c r="K21" s="36"/>
-      <c r="L21" s="37"/>
-      <c r="M21" s="37"/>
-      <c r="N21" s="38"/>
-      <c r="O21" s="37"/>
-      <c r="P21" s="39"/>
-      <c r="Q21" s="34"/>
-      <c r="R21" s="38"/>
-      <c r="S21" s="38"/>
-      <c r="T21" s="35"/>
-      <c r="U21" s="35"/>
-      <c r="V21" s="37"/>
-      <c r="W21" s="37"/>
-      <c r="X21" s="37"/>
-      <c r="Y21" s="40"/>
-      <c r="Z21" s="38"/>
-      <c r="AA21" s="41"/>
-      <c r="AB21" s="42"/>
-      <c r="AC21" s="42"/>
-      <c r="AD21" s="38"/>
-      <c r="AE21" s="38"/>
-    </row>
-    <row r="22" spans="1:31" ht="15.95" hidden="1" customHeight="1">
-      <c r="A22" s="34"/>
-      <c r="B22" s="34"/>
-      <c r="C22" s="35"/>
-      <c r="D22" s="35"/>
-      <c r="E22" s="130"/>
-      <c r="F22" s="131"/>
-      <c r="G22" s="36"/>
-      <c r="H22" s="36"/>
-      <c r="I22" s="37"/>
-      <c r="J22" s="37"/>
-      <c r="K22" s="36"/>
-      <c r="L22" s="37"/>
-      <c r="M22" s="37"/>
-      <c r="N22" s="38"/>
-      <c r="O22" s="37"/>
-      <c r="P22" s="39"/>
-      <c r="Q22" s="34"/>
-      <c r="R22" s="38"/>
-      <c r="S22" s="38"/>
-      <c r="T22" s="35"/>
-      <c r="U22" s="35"/>
-      <c r="V22" s="37"/>
-      <c r="W22" s="37"/>
-      <c r="X22" s="37"/>
-      <c r="Y22" s="40"/>
-      <c r="Z22" s="38"/>
-      <c r="AA22" s="41"/>
-      <c r="AB22" s="42"/>
-      <c r="AC22" s="42"/>
-      <c r="AD22" s="38"/>
-      <c r="AE22" s="38"/>
-    </row>
-    <row r="23" spans="1:31" ht="15.95" hidden="1" customHeight="1">
-      <c r="A23" s="34"/>
-      <c r="B23" s="34"/>
-      <c r="C23" s="35"/>
-      <c r="D23" s="35"/>
-      <c r="E23" s="130"/>
-      <c r="F23" s="131"/>
-      <c r="G23" s="36"/>
-      <c r="H23" s="36"/>
-      <c r="I23" s="37"/>
-      <c r="J23" s="37"/>
-      <c r="K23" s="36"/>
-      <c r="L23" s="37"/>
-      <c r="M23" s="37"/>
-      <c r="N23" s="38"/>
-      <c r="O23" s="37"/>
-      <c r="P23" s="39"/>
-      <c r="Q23" s="34"/>
-      <c r="R23" s="38"/>
-      <c r="S23" s="38"/>
-      <c r="T23" s="35"/>
-      <c r="U23" s="35"/>
-      <c r="V23" s="37"/>
-      <c r="W23" s="37"/>
-      <c r="X23" s="37"/>
-      <c r="Y23" s="40"/>
-      <c r="Z23" s="38"/>
-      <c r="AA23" s="41"/>
-      <c r="AB23" s="42"/>
-      <c r="AC23" s="42"/>
-      <c r="AD23" s="38"/>
-      <c r="AE23" s="38"/>
-    </row>
-    <row r="24" spans="1:31" ht="15.95" hidden="1" customHeight="1">
-      <c r="A24" s="34"/>
-      <c r="B24" s="34"/>
-      <c r="C24" s="35"/>
-      <c r="D24" s="35"/>
-      <c r="E24" s="130"/>
-      <c r="F24" s="131"/>
-      <c r="G24" s="36"/>
-      <c r="H24" s="36"/>
-      <c r="I24" s="37"/>
-      <c r="J24" s="37"/>
-      <c r="K24" s="36"/>
-      <c r="L24" s="37"/>
-      <c r="M24" s="37"/>
-      <c r="N24" s="38"/>
-      <c r="O24" s="37"/>
-      <c r="P24" s="39"/>
-      <c r="Q24" s="34"/>
-      <c r="R24" s="38"/>
-      <c r="S24" s="38"/>
-      <c r="T24" s="35"/>
-      <c r="U24" s="35"/>
-      <c r="V24" s="37"/>
-      <c r="W24" s="37"/>
-      <c r="X24" s="37"/>
-      <c r="Y24" s="40"/>
-      <c r="Z24" s="38"/>
-      <c r="AA24" s="41"/>
-      <c r="AB24" s="42"/>
-      <c r="AC24" s="42"/>
-      <c r="AD24" s="38"/>
-      <c r="AE24" s="38"/>
-    </row>
-    <row r="25" spans="1:31" ht="15.95" hidden="1" customHeight="1">
-      <c r="A25" s="34"/>
-      <c r="B25" s="34"/>
-      <c r="C25" s="35"/>
-      <c r="D25" s="35"/>
-      <c r="E25" s="130"/>
-      <c r="F25" s="131"/>
-      <c r="G25" s="36"/>
-      <c r="H25" s="36"/>
-      <c r="I25" s="37"/>
-      <c r="J25" s="37"/>
-      <c r="K25" s="36"/>
-      <c r="L25" s="37"/>
-      <c r="M25" s="37"/>
-      <c r="N25" s="38"/>
-      <c r="O25" s="37"/>
-      <c r="P25" s="39"/>
-      <c r="Q25" s="34"/>
-      <c r="R25" s="38"/>
-      <c r="S25" s="38"/>
-      <c r="T25" s="35"/>
-      <c r="U25" s="35"/>
-      <c r="V25" s="37"/>
-      <c r="W25" s="37"/>
-      <c r="X25" s="37"/>
-      <c r="Y25" s="40"/>
-      <c r="Z25" s="38"/>
-      <c r="AA25" s="41"/>
-      <c r="AB25" s="42"/>
-      <c r="AC25" s="42"/>
-      <c r="AD25" s="38"/>
-      <c r="AE25" s="38"/>
-    </row>
-    <row r="26" spans="1:31" ht="15.95" hidden="1" customHeight="1">
-      <c r="A26" s="34"/>
-      <c r="B26" s="34"/>
-      <c r="C26" s="35"/>
-      <c r="D26" s="35"/>
-      <c r="E26" s="130"/>
-      <c r="F26" s="131"/>
-      <c r="G26" s="36"/>
-      <c r="H26" s="36"/>
-      <c r="I26" s="37"/>
-      <c r="J26" s="37"/>
-      <c r="K26" s="36"/>
-      <c r="L26" s="37"/>
-      <c r="M26" s="37"/>
-      <c r="N26" s="38"/>
-      <c r="O26" s="37"/>
-      <c r="P26" s="39"/>
-      <c r="Q26" s="34"/>
-      <c r="R26" s="38"/>
-      <c r="S26" s="38"/>
-      <c r="T26" s="35"/>
-      <c r="U26" s="35"/>
-      <c r="V26" s="37"/>
-      <c r="W26" s="37"/>
-      <c r="X26" s="37"/>
-      <c r="Y26" s="40"/>
-      <c r="Z26" s="38"/>
-      <c r="AA26" s="41"/>
-      <c r="AB26" s="42"/>
-      <c r="AC26" s="42"/>
-      <c r="AD26" s="38"/>
-      <c r="AE26" s="38"/>
-    </row>
-    <row r="27" spans="1:31" ht="15.95" hidden="1" customHeight="1">
-      <c r="A27" s="34"/>
-      <c r="B27" s="34"/>
-      <c r="C27" s="35"/>
-      <c r="D27" s="35"/>
-      <c r="E27" s="130"/>
-      <c r="F27" s="131"/>
-      <c r="G27" s="36"/>
-      <c r="H27" s="36"/>
-      <c r="I27" s="37"/>
-      <c r="J27" s="37"/>
-      <c r="K27" s="36"/>
-      <c r="L27" s="37"/>
-      <c r="M27" s="37"/>
-      <c r="N27" s="38"/>
-      <c r="O27" s="37"/>
-      <c r="P27" s="39"/>
-      <c r="Q27" s="34"/>
-      <c r="R27" s="38"/>
-      <c r="S27" s="38"/>
-      <c r="T27" s="35"/>
-      <c r="U27" s="35"/>
-      <c r="V27" s="37"/>
-      <c r="W27" s="37"/>
-      <c r="X27" s="37"/>
-      <c r="Y27" s="40"/>
-      <c r="Z27" s="38"/>
-      <c r="AA27" s="41"/>
-      <c r="AB27" s="42"/>
-      <c r="AC27" s="42"/>
-      <c r="AD27" s="38"/>
-      <c r="AE27" s="38"/>
-    </row>
-    <row r="28" spans="1:31" ht="15.95" hidden="1" customHeight="1">
-      <c r="A28" s="34"/>
-      <c r="B28" s="34"/>
-      <c r="C28" s="35"/>
-      <c r="D28" s="35"/>
-      <c r="E28" s="130"/>
-      <c r="F28" s="131"/>
-      <c r="G28" s="36"/>
-      <c r="H28" s="36"/>
-      <c r="I28" s="37"/>
-      <c r="J28" s="37"/>
-      <c r="K28" s="36"/>
-      <c r="L28" s="37"/>
-      <c r="M28" s="37"/>
-      <c r="N28" s="38"/>
-      <c r="O28" s="37"/>
-      <c r="P28" s="39"/>
-      <c r="Q28" s="34"/>
-      <c r="R28" s="38"/>
-      <c r="S28" s="38"/>
-      <c r="T28" s="35"/>
-      <c r="U28" s="35"/>
-      <c r="V28" s="37"/>
-      <c r="W28" s="37"/>
-      <c r="X28" s="37"/>
-      <c r="Y28" s="40"/>
-      <c r="Z28" s="38"/>
-      <c r="AA28" s="41"/>
-      <c r="AB28" s="42"/>
-      <c r="AC28" s="42"/>
-      <c r="AD28" s="38"/>
-      <c r="AE28" s="38"/>
-    </row>
-    <row r="29" spans="1:31" ht="15.95" hidden="1" customHeight="1">
-      <c r="A29" s="34"/>
-      <c r="B29" s="34"/>
-      <c r="C29" s="35"/>
-      <c r="D29" s="35"/>
-      <c r="E29" s="130"/>
-      <c r="F29" s="131"/>
-      <c r="G29" s="36"/>
-      <c r="H29" s="36"/>
-      <c r="I29" s="37"/>
-      <c r="J29" s="37"/>
-      <c r="K29" s="36"/>
-      <c r="L29" s="37"/>
-      <c r="M29" s="37"/>
-      <c r="N29" s="38"/>
-      <c r="O29" s="37"/>
-      <c r="P29" s="39"/>
-      <c r="Q29" s="34"/>
-      <c r="R29" s="38"/>
-      <c r="S29" s="38"/>
-      <c r="T29" s="35"/>
-      <c r="U29" s="35"/>
-      <c r="V29" s="37"/>
-      <c r="W29" s="37"/>
-      <c r="X29" s="37"/>
-      <c r="Y29" s="40"/>
-      <c r="Z29" s="38"/>
-      <c r="AA29" s="41"/>
-      <c r="AB29" s="42"/>
-      <c r="AC29" s="42"/>
-      <c r="AD29" s="38"/>
-      <c r="AE29" s="38"/>
-    </row>
-    <row r="30" spans="1:31" ht="15.95" hidden="1" customHeight="1">
-      <c r="A30" s="34"/>
-      <c r="B30" s="34"/>
-      <c r="C30" s="35"/>
-      <c r="D30" s="35"/>
-      <c r="E30" s="130"/>
-      <c r="F30" s="131"/>
-      <c r="G30" s="36"/>
-      <c r="H30" s="36"/>
-      <c r="I30" s="37"/>
-      <c r="J30" s="37"/>
-      <c r="K30" s="36"/>
-      <c r="L30" s="37"/>
-      <c r="M30" s="37"/>
-      <c r="N30" s="38"/>
-      <c r="O30" s="37"/>
-      <c r="P30" s="39"/>
-      <c r="Q30" s="34"/>
-      <c r="R30" s="38"/>
-      <c r="S30" s="38"/>
-      <c r="T30" s="35"/>
-      <c r="U30" s="35"/>
-      <c r="V30" s="37"/>
-      <c r="W30" s="37"/>
-      <c r="X30" s="37"/>
-      <c r="Y30" s="40"/>
-      <c r="Z30" s="38"/>
-      <c r="AA30" s="41"/>
-      <c r="AB30" s="42"/>
-      <c r="AC30" s="42"/>
-      <c r="AD30" s="38"/>
-      <c r="AE30" s="38"/>
-    </row>
-    <row r="31" spans="1:31" ht="15.95" hidden="1" customHeight="1">
-      <c r="A31" s="34"/>
-      <c r="B31" s="34"/>
-      <c r="C31" s="35"/>
-      <c r="D31" s="35"/>
-      <c r="E31" s="130"/>
-      <c r="F31" s="131"/>
-      <c r="G31" s="36"/>
-      <c r="H31" s="36"/>
-      <c r="I31" s="37"/>
-      <c r="J31" s="37"/>
-      <c r="K31" s="36"/>
-      <c r="L31" s="37"/>
-      <c r="M31" s="37"/>
-      <c r="N31" s="38"/>
-      <c r="O31" s="37"/>
-      <c r="P31" s="39"/>
-      <c r="Q31" s="34"/>
-      <c r="R31" s="38"/>
-      <c r="S31" s="38"/>
-      <c r="T31" s="35"/>
-      <c r="U31" s="35"/>
-      <c r="V31" s="37"/>
-      <c r="W31" s="37"/>
-      <c r="X31" s="37"/>
-      <c r="Y31" s="40"/>
-      <c r="Z31" s="38"/>
-      <c r="AA31" s="41"/>
-      <c r="AB31" s="42"/>
-      <c r="AC31" s="42"/>
-      <c r="AD31" s="38"/>
-      <c r="AE31" s="38"/>
-    </row>
-    <row r="32" spans="1:31" ht="15.95" hidden="1" customHeight="1">
-      <c r="A32" s="34"/>
-      <c r="B32" s="34"/>
-      <c r="C32" s="35"/>
-      <c r="D32" s="35"/>
-      <c r="E32" s="130"/>
-      <c r="F32" s="131"/>
-      <c r="G32" s="36"/>
-      <c r="H32" s="36"/>
-      <c r="I32" s="37"/>
-      <c r="J32" s="37"/>
-      <c r="K32" s="36"/>
-      <c r="L32" s="37"/>
-      <c r="M32" s="37"/>
-      <c r="N32" s="38"/>
-      <c r="O32" s="37"/>
-      <c r="P32" s="39"/>
-      <c r="Q32" s="34"/>
-      <c r="R32" s="38"/>
-      <c r="S32" s="38"/>
-      <c r="T32" s="35"/>
-      <c r="U32" s="35"/>
-      <c r="V32" s="37"/>
-      <c r="W32" s="37"/>
-      <c r="X32" s="37"/>
-      <c r="Y32" s="40"/>
-      <c r="Z32" s="38"/>
-      <c r="AA32" s="41"/>
-      <c r="AB32" s="42"/>
-      <c r="AC32" s="42"/>
-      <c r="AD32" s="38"/>
-      <c r="AE32" s="38"/>
-    </row>
-    <row r="33" spans="1:31" ht="15.95" hidden="1" customHeight="1">
-      <c r="A33" s="34"/>
-      <c r="B33" s="34"/>
-      <c r="C33" s="35"/>
-      <c r="D33" s="35"/>
-      <c r="E33" s="130"/>
-      <c r="F33" s="131"/>
-      <c r="G33" s="36"/>
-      <c r="H33" s="36"/>
-      <c r="I33" s="37"/>
-      <c r="J33" s="37"/>
-      <c r="K33" s="36"/>
-      <c r="L33" s="37"/>
-      <c r="M33" s="37"/>
-      <c r="N33" s="38"/>
-      <c r="O33" s="37"/>
-      <c r="P33" s="39"/>
-      <c r="Q33" s="34"/>
-      <c r="R33" s="38"/>
-      <c r="S33" s="38"/>
-      <c r="T33" s="35"/>
-      <c r="U33" s="35"/>
-      <c r="V33" s="37"/>
-      <c r="W33" s="37"/>
-      <c r="X33" s="37"/>
-      <c r="Y33" s="40"/>
-      <c r="Z33" s="38"/>
-      <c r="AA33" s="41"/>
-      <c r="AB33" s="42"/>
-      <c r="AC33" s="42"/>
-      <c r="AD33" s="38"/>
-      <c r="AE33" s="38"/>
-    </row>
-    <row r="34" spans="1:31" ht="15.95" hidden="1" customHeight="1">
-      <c r="A34" s="34"/>
-      <c r="B34" s="34"/>
-      <c r="C34" s="35"/>
-      <c r="D34" s="35"/>
-      <c r="E34" s="130"/>
-      <c r="F34" s="131"/>
-      <c r="G34" s="36"/>
-      <c r="H34" s="36"/>
-      <c r="I34" s="37"/>
-      <c r="J34" s="37"/>
-      <c r="K34" s="36"/>
-      <c r="L34" s="37"/>
-      <c r="M34" s="37"/>
-      <c r="N34" s="38"/>
-      <c r="O34" s="37"/>
-      <c r="P34" s="39"/>
-      <c r="Q34" s="34"/>
-      <c r="R34" s="38"/>
-      <c r="S34" s="38"/>
-      <c r="T34" s="35"/>
-      <c r="U34" s="35"/>
-      <c r="V34" s="37"/>
-      <c r="W34" s="37"/>
-      <c r="X34" s="37"/>
-      <c r="Y34" s="40"/>
-      <c r="Z34" s="38"/>
-      <c r="AA34" s="41"/>
-      <c r="AB34" s="42"/>
-      <c r="AC34" s="42"/>
-      <c r="AD34" s="38"/>
-      <c r="AE34" s="38"/>
-    </row>
-    <row r="35" spans="1:31" ht="15.95" hidden="1" customHeight="1">
-      <c r="A35" s="34"/>
-      <c r="B35" s="34"/>
-      <c r="C35" s="35"/>
-      <c r="D35" s="35"/>
-      <c r="E35" s="130"/>
-      <c r="F35" s="131"/>
-      <c r="G35" s="36"/>
-      <c r="H35" s="36"/>
-      <c r="I35" s="37"/>
-      <c r="J35" s="37"/>
-      <c r="K35" s="36"/>
-      <c r="L35" s="37"/>
-      <c r="M35" s="37"/>
-      <c r="N35" s="38"/>
-      <c r="O35" s="37"/>
-      <c r="P35" s="39"/>
-      <c r="Q35" s="34"/>
-      <c r="R35" s="38"/>
-      <c r="S35" s="38"/>
-      <c r="T35" s="35"/>
-      <c r="U35" s="35"/>
-      <c r="V35" s="37"/>
-      <c r="W35" s="37"/>
-      <c r="X35" s="37"/>
-      <c r="Y35" s="40"/>
-      <c r="Z35" s="38"/>
-      <c r="AA35" s="41"/>
-      <c r="AB35" s="42"/>
-      <c r="AC35" s="42"/>
-      <c r="AD35" s="38"/>
-      <c r="AE35" s="38"/>
-    </row>
-    <row r="36" spans="1:31" ht="15.95" hidden="1" customHeight="1">
-      <c r="A36" s="34"/>
-      <c r="B36" s="34"/>
-      <c r="C36" s="35"/>
-      <c r="D36" s="35"/>
-      <c r="E36" s="130"/>
-      <c r="F36" s="131"/>
-      <c r="G36" s="36"/>
-      <c r="H36" s="36"/>
-      <c r="I36" s="37"/>
-      <c r="J36" s="37"/>
-      <c r="K36" s="36"/>
-      <c r="L36" s="37"/>
-      <c r="M36" s="37"/>
-      <c r="N36" s="38"/>
-      <c r="O36" s="37"/>
-      <c r="P36" s="39"/>
-      <c r="Q36" s="34"/>
-      <c r="R36" s="38"/>
-      <c r="S36" s="38"/>
-      <c r="T36" s="35"/>
-      <c r="U36" s="35"/>
-      <c r="V36" s="37"/>
-      <c r="W36" s="37"/>
-      <c r="X36" s="37"/>
-      <c r="Y36" s="40"/>
-      <c r="Z36" s="38"/>
-      <c r="AA36" s="41"/>
-      <c r="AB36" s="42"/>
-      <c r="AC36" s="42"/>
-      <c r="AD36" s="38"/>
-      <c r="AE36" s="38"/>
-    </row>
-    <row r="37" spans="1:31" ht="15.95" hidden="1" customHeight="1">
-      <c r="A37" s="34"/>
-      <c r="B37" s="34"/>
-      <c r="C37" s="35"/>
-      <c r="D37" s="35"/>
-      <c r="E37" s="130"/>
-      <c r="F37" s="131"/>
-      <c r="G37" s="36"/>
-      <c r="H37" s="36"/>
-      <c r="I37" s="37"/>
-      <c r="J37" s="37"/>
-      <c r="K37" s="36"/>
-      <c r="L37" s="37"/>
-      <c r="M37" s="37"/>
-      <c r="N37" s="38"/>
-      <c r="O37" s="37"/>
-      <c r="P37" s="39"/>
-      <c r="Q37" s="34"/>
-      <c r="R37" s="38"/>
-      <c r="S37" s="38"/>
-      <c r="T37" s="35"/>
-      <c r="U37" s="35"/>
-      <c r="V37" s="37"/>
-      <c r="W37" s="37"/>
-      <c r="X37" s="37"/>
-      <c r="Y37" s="40"/>
-      <c r="Z37" s="38"/>
-      <c r="AA37" s="41"/>
-      <c r="AB37" s="42"/>
-      <c r="AC37" s="42"/>
-      <c r="AD37" s="38"/>
-      <c r="AE37" s="38"/>
-    </row>
-    <row r="38" spans="1:31" ht="15.95" hidden="1" customHeight="1">
-      <c r="A38" s="34"/>
-      <c r="B38" s="34"/>
-      <c r="C38" s="35"/>
-      <c r="D38" s="35"/>
-      <c r="E38" s="130"/>
-      <c r="F38" s="131"/>
-      <c r="G38" s="36"/>
-      <c r="H38" s="36"/>
-      <c r="I38" s="37"/>
-      <c r="J38" s="37"/>
-      <c r="K38" s="36"/>
-      <c r="L38" s="37"/>
-      <c r="M38" s="37"/>
-      <c r="N38" s="38"/>
-      <c r="O38" s="37"/>
-      <c r="P38" s="39"/>
-      <c r="Q38" s="34"/>
-      <c r="R38" s="38"/>
-      <c r="S38" s="38"/>
-      <c r="T38" s="35"/>
-      <c r="U38" s="35"/>
-      <c r="V38" s="37"/>
-      <c r="W38" s="37"/>
-      <c r="X38" s="37"/>
-      <c r="Y38" s="40"/>
-      <c r="Z38" s="38"/>
-      <c r="AA38" s="41"/>
-      <c r="AB38" s="42"/>
-      <c r="AC38" s="42"/>
-      <c r="AD38" s="38"/>
-      <c r="AE38" s="38"/>
-    </row>
-    <row r="39" spans="1:31" ht="15.95" hidden="1" customHeight="1">
-      <c r="A39" s="34"/>
-      <c r="B39" s="34"/>
-      <c r="C39" s="35"/>
-      <c r="D39" s="35"/>
-      <c r="E39" s="130"/>
-      <c r="F39" s="131"/>
-      <c r="G39" s="36"/>
-      <c r="H39" s="36"/>
-      <c r="I39" s="37"/>
-      <c r="J39" s="37"/>
-      <c r="K39" s="36"/>
-      <c r="L39" s="37"/>
-      <c r="M39" s="37"/>
-      <c r="N39" s="38"/>
-      <c r="O39" s="37"/>
-      <c r="P39" s="39"/>
-      <c r="Q39" s="34"/>
-      <c r="R39" s="38"/>
-      <c r="S39" s="38"/>
-      <c r="T39" s="35"/>
-      <c r="U39" s="35"/>
-      <c r="V39" s="37"/>
-      <c r="W39" s="37"/>
-      <c r="X39" s="37"/>
-      <c r="Y39" s="40"/>
-      <c r="Z39" s="38"/>
-      <c r="AA39" s="41"/>
-      <c r="AB39" s="42"/>
-      <c r="AC39" s="42"/>
-      <c r="AD39" s="38"/>
-      <c r="AE39" s="38"/>
-    </row>
-    <row r="40" spans="1:31" ht="15.95" hidden="1" customHeight="1">
-      <c r="A40" s="34"/>
-      <c r="B40" s="34"/>
-      <c r="C40" s="35"/>
-      <c r="D40" s="35"/>
-      <c r="E40" s="130"/>
-      <c r="F40" s="131"/>
-      <c r="G40" s="36"/>
-      <c r="H40" s="36"/>
-      <c r="I40" s="37"/>
-      <c r="J40" s="37"/>
-      <c r="K40" s="36"/>
-      <c r="L40" s="37"/>
-      <c r="M40" s="37"/>
-      <c r="N40" s="38"/>
-      <c r="O40" s="37"/>
-      <c r="P40" s="39"/>
-      <c r="Q40" s="34"/>
-      <c r="R40" s="38"/>
-      <c r="S40" s="38"/>
-      <c r="T40" s="35"/>
-      <c r="U40" s="35"/>
-      <c r="V40" s="37"/>
-      <c r="W40" s="37"/>
-      <c r="X40" s="37"/>
-      <c r="Y40" s="40"/>
-      <c r="Z40" s="38"/>
-      <c r="AA40" s="41"/>
-      <c r="AB40" s="42"/>
-      <c r="AC40" s="42"/>
-      <c r="AD40" s="38"/>
-      <c r="AE40" s="38"/>
-    </row>
-    <row r="41" spans="1:31" ht="15.95" hidden="1" customHeight="1">
-      <c r="A41" s="34"/>
-      <c r="B41" s="34"/>
-      <c r="C41" s="35"/>
-      <c r="D41" s="35"/>
-      <c r="E41" s="130"/>
-      <c r="F41" s="131"/>
-      <c r="G41" s="36"/>
-      <c r="H41" s="36"/>
-      <c r="I41" s="37"/>
-      <c r="J41" s="37"/>
-      <c r="K41" s="36"/>
-      <c r="L41" s="37"/>
-      <c r="M41" s="37"/>
-      <c r="N41" s="38"/>
-      <c r="O41" s="37"/>
-      <c r="P41" s="39"/>
-      <c r="Q41" s="34"/>
-      <c r="R41" s="38"/>
-      <c r="S41" s="38"/>
-      <c r="T41" s="35"/>
-      <c r="U41" s="35"/>
-      <c r="V41" s="37"/>
-      <c r="W41" s="37"/>
-      <c r="X41" s="37"/>
-      <c r="Y41" s="40"/>
-      <c r="Z41" s="38"/>
-      <c r="AA41" s="41"/>
-      <c r="AB41" s="42"/>
-      <c r="AC41" s="42"/>
-      <c r="AD41" s="38"/>
-      <c r="AE41" s="38"/>
-    </row>
-    <row r="42" spans="1:31" ht="15.95" hidden="1" customHeight="1">
-      <c r="A42" s="34"/>
-      <c r="B42" s="34"/>
-      <c r="C42" s="35"/>
-      <c r="D42" s="35"/>
-      <c r="E42" s="130"/>
-      <c r="F42" s="131"/>
-      <c r="G42" s="36"/>
-      <c r="H42" s="36"/>
-      <c r="I42" s="37"/>
-      <c r="J42" s="37"/>
-      <c r="K42" s="36"/>
-      <c r="L42" s="37"/>
-      <c r="M42" s="37"/>
-      <c r="N42" s="38"/>
-      <c r="O42" s="37"/>
-      <c r="P42" s="39"/>
-      <c r="Q42" s="34"/>
-      <c r="R42" s="38"/>
-      <c r="S42" s="38"/>
-      <c r="T42" s="35"/>
-      <c r="U42" s="35"/>
-      <c r="V42" s="37"/>
-      <c r="W42" s="37"/>
-      <c r="X42" s="37"/>
-      <c r="Y42" s="40"/>
-      <c r="Z42" s="38"/>
-      <c r="AA42" s="41"/>
-      <c r="AB42" s="42"/>
-      <c r="AC42" s="42"/>
-      <c r="AD42" s="38"/>
-      <c r="AE42" s="38"/>
-    </row>
-    <row r="43" spans="1:31" ht="15.95" hidden="1" customHeight="1">
-      <c r="A43" s="43"/>
-      <c r="B43" s="43"/>
-      <c r="C43" s="44"/>
-      <c r="D43" s="44"/>
-      <c r="E43" s="132"/>
-      <c r="F43" s="133"/>
-      <c r="G43" s="45"/>
-      <c r="H43" s="45"/>
-      <c r="I43" s="44"/>
-      <c r="J43" s="44"/>
-      <c r="K43" s="45"/>
-      <c r="L43" s="44"/>
-      <c r="M43" s="44"/>
-      <c r="N43" s="43"/>
-      <c r="O43" s="44"/>
-      <c r="P43" s="46"/>
-      <c r="Q43" s="43"/>
-      <c r="R43" s="43"/>
-      <c r="S43" s="43"/>
-      <c r="T43" s="44"/>
-      <c r="U43" s="44"/>
-      <c r="V43" s="44"/>
-      <c r="W43" s="44"/>
-      <c r="X43" s="44"/>
-      <c r="Y43" s="40"/>
-      <c r="Z43" s="43"/>
-      <c r="AA43" s="46"/>
-      <c r="AB43" s="47"/>
-      <c r="AC43" s="47"/>
-      <c r="AD43" s="43"/>
-      <c r="AE43" s="43"/>
-    </row>
-    <row r="44" spans="1:31">
-      <c r="A44" s="48" t="s">
+    <row r="14" spans="1:30">
+      <c r="A14" s="48" t="s">
         <v>67</v>
       </c>
-      <c r="B44" s="48" t="s">
-        <v>23</v>
-      </c>
-      <c r="C44" s="49">
-        <v>0</v>
-      </c>
-      <c r="D44" s="49">
-        <v>0</v>
-      </c>
-      <c r="E44" s="137"/>
-      <c r="F44" s="138"/>
-      <c r="G44" s="50">
-        <v>0</v>
-      </c>
-      <c r="H44" s="50">
-        <v>0</v>
-      </c>
-      <c r="I44" s="49"/>
-      <c r="J44" s="49"/>
-      <c r="K44" s="50">
-        <v>0</v>
-      </c>
-      <c r="L44" s="49"/>
-      <c r="M44" s="49"/>
-      <c r="N44" s="48">
-        <v>0</v>
-      </c>
-      <c r="O44" s="49"/>
-      <c r="P44" s="51"/>
-      <c r="Q44" s="48"/>
-      <c r="R44" s="48"/>
-      <c r="S44" s="48"/>
-      <c r="T44" s="49">
-        <v>0</v>
-      </c>
-      <c r="U44" s="49">
-        <v>0</v>
-      </c>
-      <c r="V44" s="49">
-        <v>0</v>
-      </c>
-      <c r="W44" s="49">
-        <v>0</v>
-      </c>
-      <c r="X44" s="49">
-        <v>0</v>
-      </c>
-      <c r="Y44" s="52" t="s">
-        <v>23</v>
-      </c>
-      <c r="Z44" s="48"/>
-      <c r="AA44" s="51"/>
-      <c r="AB44" s="53"/>
-      <c r="AC44" s="53"/>
-      <c r="AD44" s="48"/>
-      <c r="AE44" s="48"/>
+      <c r="B14" s="48" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="49">
+        <v>0</v>
+      </c>
+      <c r="D14" s="49">
+        <v>0</v>
+      </c>
+      <c r="E14" s="109"/>
+      <c r="F14" s="50">
+        <v>0</v>
+      </c>
+      <c r="G14" s="50">
+        <v>0</v>
+      </c>
+      <c r="H14" s="49"/>
+      <c r="I14" s="49"/>
+      <c r="J14" s="50">
+        <v>0</v>
+      </c>
+      <c r="K14" s="49"/>
+      <c r="L14" s="49"/>
+      <c r="M14" s="48">
+        <v>0</v>
+      </c>
+      <c r="N14" s="49"/>
+      <c r="O14" s="51"/>
+      <c r="P14" s="48"/>
+      <c r="Q14" s="48"/>
+      <c r="R14" s="48"/>
+      <c r="S14" s="49">
+        <v>0</v>
+      </c>
+      <c r="T14" s="49">
+        <v>0</v>
+      </c>
+      <c r="U14" s="49">
+        <v>0</v>
+      </c>
+      <c r="V14" s="49">
+        <v>0</v>
+      </c>
+      <c r="W14" s="49">
+        <v>0</v>
+      </c>
+      <c r="X14" s="52" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y14" s="48"/>
+      <c r="Z14" s="51"/>
+      <c r="AA14" s="53"/>
+      <c r="AB14" s="53"/>
+      <c r="AC14" s="48"/>
+      <c r="AD14" s="48"/>
     </row>
   </sheetData>
-  <mergeCells count="53">
-    <mergeCell ref="E40:F40"/>
-    <mergeCell ref="E41:F41"/>
-    <mergeCell ref="E42:F42"/>
-    <mergeCell ref="E43:F43"/>
-    <mergeCell ref="E44:F44"/>
-    <mergeCell ref="E39:F39"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="E13:F13"/>
+  <mergeCells count="16">
     <mergeCell ref="A7:B7"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="C7:F7"/>
     <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:G5"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="I5:J5"/>
     <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:G6"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="C6:F6"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="I4:J4"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A3:E3"/>
     <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:G4"/>
-    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="G4:H4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3858,10 +2897,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AE15"/>
+  <sheetPr codeName="Sheet3"/>
+  <dimension ref="A1:AD15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -3871,16 +2911,15 @@
     <col min="3" max="3" width="15.7109375" style="57" customWidth="1"/>
     <col min="4" max="4" width="13.7109375" style="57" customWidth="1"/>
     <col min="5" max="5" width="13.28515625" style="57" customWidth="1"/>
-    <col min="6" max="6" width="1" style="57" customWidth="1"/>
-    <col min="7" max="18" width="13.7109375" style="57" customWidth="1"/>
-    <col min="19" max="19" width="19.85546875" style="57" customWidth="1"/>
-    <col min="20" max="24" width="13.7109375" style="57" customWidth="1"/>
-    <col min="25" max="25" width="2.7109375" style="57" customWidth="1"/>
-    <col min="26" max="31" width="13.7109375" style="57" customWidth="1"/>
-    <col min="32" max="16384" width="9.140625" style="57"/>
+    <col min="6" max="17" width="13.7109375" style="57" customWidth="1"/>
+    <col min="18" max="18" width="19.85546875" style="57" customWidth="1"/>
+    <col min="19" max="23" width="13.7109375" style="57" customWidth="1"/>
+    <col min="24" max="24" width="2.7109375" style="57" customWidth="1"/>
+    <col min="25" max="30" width="13.7109375" style="57" customWidth="1"/>
+    <col min="31" max="16384" width="9.140625" style="57"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" ht="21" customHeight="1">
+    <row r="1" spans="1:30" ht="21" customHeight="1">
       <c r="A1" s="54" t="s">
         <v>12</v>
       </c>
@@ -3913,9 +2952,8 @@
       <c r="AB1" s="56"/>
       <c r="AC1" s="56"/>
       <c r="AD1" s="56"/>
-      <c r="AE1" s="56"/>
-    </row>
-    <row r="2" spans="1:31" ht="6.95" customHeight="1">
+    </row>
+    <row r="2" spans="1:30" ht="6.95" customHeight="1">
       <c r="A2" s="56"/>
       <c r="B2" s="56"/>
       <c r="C2" s="56"/>
@@ -3946,9 +2984,8 @@
       <c r="AB2" s="56"/>
       <c r="AC2" s="56"/>
       <c r="AD2" s="56"/>
-      <c r="AE2" s="56"/>
-    </row>
-    <row r="3" spans="1:31" ht="21" customHeight="1">
+    </row>
+    <row r="3" spans="1:30" ht="21" customHeight="1">
       <c r="A3" s="58" t="s">
         <v>68</v>
       </c>
@@ -3981,9 +3018,8 @@
       <c r="AB3" s="56"/>
       <c r="AC3" s="56"/>
       <c r="AD3" s="56"/>
-      <c r="AE3" s="56"/>
-    </row>
-    <row r="4" spans="1:31" ht="18" customHeight="1">
+    </row>
+    <row r="4" spans="1:30" ht="18" customHeight="1">
       <c r="A4" s="60" t="s">
         <v>14</v>
       </c>
@@ -3994,13 +3030,13 @@
       <c r="D4" s="62"/>
       <c r="E4" s="62"/>
       <c r="F4" s="62"/>
-      <c r="G4" s="62"/>
-      <c r="H4" s="139" t="s">
+      <c r="G4" s="133" t="s">
         <v>16</v>
       </c>
-      <c r="I4" s="139"/>
-      <c r="J4" s="140"/>
-      <c r="K4" s="140"/>
+      <c r="H4" s="133"/>
+      <c r="I4" s="134"/>
+      <c r="J4" s="134"/>
+      <c r="K4" s="56"/>
       <c r="L4" s="56"/>
       <c r="M4" s="56"/>
       <c r="N4" s="56"/>
@@ -4020,9 +3056,8 @@
       <c r="AB4" s="56"/>
       <c r="AC4" s="56"/>
       <c r="AD4" s="56"/>
-      <c r="AE4" s="56"/>
-    </row>
-    <row r="5" spans="1:31" ht="17.100000000000001" customHeight="1">
+    </row>
+    <row r="5" spans="1:30" ht="17.100000000000001" customHeight="1">
       <c r="A5" s="60" t="s">
         <v>18</v>
       </c>
@@ -4031,13 +3066,13 @@
       <c r="D5" s="63"/>
       <c r="E5" s="63"/>
       <c r="F5" s="63"/>
-      <c r="G5" s="63"/>
-      <c r="H5" s="139" t="s">
+      <c r="G5" s="133" t="s">
         <v>20</v>
       </c>
-      <c r="I5" s="139"/>
-      <c r="J5" s="140"/>
-      <c r="K5" s="140"/>
+      <c r="H5" s="133"/>
+      <c r="I5" s="134"/>
+      <c r="J5" s="134"/>
+      <c r="K5" s="56"/>
       <c r="L5" s="56"/>
       <c r="M5" s="56"/>
       <c r="N5" s="56"/>
@@ -4057,9 +3092,8 @@
       <c r="AB5" s="56"/>
       <c r="AC5" s="56"/>
       <c r="AD5" s="56"/>
-      <c r="AE5" s="56"/>
-    </row>
-    <row r="6" spans="1:31" ht="18.95" customHeight="1">
+    </row>
+    <row r="6" spans="1:30" ht="18.95" customHeight="1">
       <c r="A6" s="60" t="s">
         <v>22</v>
       </c>
@@ -4068,15 +3102,17 @@
       <c r="D6" s="64"/>
       <c r="E6" s="64"/>
       <c r="F6" s="64"/>
-      <c r="G6" s="64"/>
-      <c r="H6" s="141" t="s">
-        <v>23</v>
-      </c>
-      <c r="I6" s="141"/>
-      <c r="J6" s="141" t="s">
-        <v>23</v>
-      </c>
-      <c r="K6" s="141"/>
+      <c r="G6" s="135" t="s">
+        <v>23</v>
+      </c>
+      <c r="H6" s="135"/>
+      <c r="I6" s="135" t="s">
+        <v>23</v>
+      </c>
+      <c r="J6" s="135"/>
+      <c r="K6" s="65" t="s">
+        <v>23</v>
+      </c>
       <c r="L6" s="65" t="s">
         <v>23</v>
       </c>
@@ -4134,18 +3170,17 @@
       <c r="AD6" s="65" t="s">
         <v>23</v>
       </c>
-      <c r="AE6" s="65" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:31">
+    </row>
+    <row r="7" spans="1:30">
       <c r="A7" s="66"/>
       <c r="B7" s="66"/>
       <c r="C7" s="66"/>
       <c r="D7" s="66"/>
       <c r="E7" s="66"/>
       <c r="F7" s="66"/>
-      <c r="G7" s="66"/>
+      <c r="G7" s="65" t="s">
+        <v>23</v>
+      </c>
       <c r="H7" s="65" t="s">
         <v>23</v>
       </c>
@@ -4215,11 +3250,8 @@
       <c r="AD7" s="65" t="s">
         <v>23</v>
       </c>
-      <c r="AE7" s="65" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:31" ht="9.9499999999999993" customHeight="1">
+    </row>
+    <row r="8" spans="1:30" ht="9.9499999999999993" customHeight="1">
       <c r="A8" s="65" t="s">
         <v>23</v>
       </c>
@@ -4235,7 +3267,9 @@
       <c r="E8" s="65" t="s">
         <v>23</v>
       </c>
-      <c r="F8" s="65"/>
+      <c r="F8" s="65" t="s">
+        <v>23</v>
+      </c>
       <c r="G8" s="65" t="s">
         <v>23</v>
       </c>
@@ -4308,11 +3342,8 @@
       <c r="AD8" s="65" t="s">
         <v>23</v>
       </c>
-      <c r="AE8" s="65" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:31" ht="21.95" customHeight="1">
+    </row>
+    <row r="9" spans="1:30" ht="21.95" customHeight="1">
       <c r="A9" s="67" t="s">
         <v>26</v>
       </c>
@@ -4328,379 +3359,373 @@
       <c r="E9" s="69" t="s">
         <v>30</v>
       </c>
-      <c r="F9" s="70"/>
+      <c r="F9" s="68" t="s">
+        <v>31</v>
+      </c>
       <c r="G9" s="68" t="s">
-        <v>31</v>
-      </c>
-      <c r="H9" s="68" t="s">
         <v>32</v>
       </c>
+      <c r="H9" s="67" t="s">
+        <v>33</v>
+      </c>
       <c r="I9" s="67" t="s">
-        <v>33</v>
-      </c>
-      <c r="J9" s="67" t="s">
         <v>34</v>
       </c>
-      <c r="K9" s="68" t="s">
+      <c r="J9" s="68" t="s">
         <v>35</v>
       </c>
+      <c r="K9" s="67" t="s">
+        <v>36</v>
+      </c>
       <c r="L9" s="67" t="s">
-        <v>36</v>
-      </c>
-      <c r="M9" s="67" t="s">
         <v>37</v>
       </c>
-      <c r="N9" s="68" t="s">
+      <c r="M9" s="68" t="s">
         <v>38</v>
       </c>
+      <c r="N9" s="67" t="s">
+        <v>39</v>
+      </c>
       <c r="O9" s="67" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="P9" s="67" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q9" s="67" t="s">
         <v>41</v>
       </c>
+      <c r="Q9" s="68" t="s">
+        <v>42</v>
+      </c>
       <c r="R9" s="68" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="S9" s="68" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="T9" s="68" t="s">
-        <v>44</v>
-      </c>
-      <c r="U9" s="68" t="s">
         <v>45</v>
       </c>
+      <c r="U9" s="67" t="s">
+        <v>46</v>
+      </c>
       <c r="V9" s="67" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="W9" s="67" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="X9" s="67" t="s">
-        <v>48</v>
-      </c>
-      <c r="Y9" s="67" t="s">
-        <v>23</v>
+        <v>23</v>
+      </c>
+      <c r="Y9" s="68" t="s">
+        <v>49</v>
       </c>
       <c r="Z9" s="68" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="AA9" s="68" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="AB9" s="68" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="AC9" s="68" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="AD9" s="68" t="s">
-        <v>52</v>
-      </c>
-      <c r="AE9" s="68" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="10" spans="1:31">
-      <c r="A10" s="83" t="s">
+    <row r="10" spans="1:30">
+      <c r="A10" s="81" t="s">
         <v>70</v>
       </c>
-      <c r="B10" s="71"/>
-      <c r="C10" s="72">
-        <v>0</v>
-      </c>
-      <c r="D10" s="72">
-        <v>0</v>
-      </c>
-      <c r="E10" s="73"/>
-      <c r="F10" s="74"/>
-      <c r="G10" s="75">
-        <v>0</v>
-      </c>
-      <c r="H10" s="75">
-        <v>0</v>
-      </c>
-      <c r="I10" s="76"/>
-      <c r="J10" s="76"/>
-      <c r="K10" s="75">
-        <v>0</v>
-      </c>
-      <c r="L10" s="76"/>
-      <c r="M10" s="76"/>
-      <c r="N10" s="77">
-        <v>0</v>
-      </c>
+      <c r="B10" s="70"/>
+      <c r="C10" s="71">
+        <v>0</v>
+      </c>
+      <c r="D10" s="71">
+        <v>0</v>
+      </c>
+      <c r="E10" s="72"/>
+      <c r="F10" s="73">
+        <v>0</v>
+      </c>
+      <c r="G10" s="73">
+        <v>0</v>
+      </c>
+      <c r="H10" s="74"/>
+      <c r="I10" s="74"/>
+      <c r="J10" s="73">
+        <v>0</v>
+      </c>
+      <c r="K10" s="74"/>
+      <c r="L10" s="74"/>
+      <c r="M10" s="75">
+        <v>0</v>
+      </c>
+      <c r="N10" s="74"/>
       <c r="O10" s="76"/>
-      <c r="P10" s="78"/>
-      <c r="Q10" s="71"/>
-      <c r="R10" s="79"/>
-      <c r="S10" s="79"/>
-      <c r="T10" s="72">
-        <v>0</v>
-      </c>
-      <c r="U10" s="72">
-        <v>0</v>
-      </c>
-      <c r="V10" s="76">
-        <v>0</v>
-      </c>
-      <c r="W10" s="76">
-        <v>0</v>
-      </c>
-      <c r="X10" s="76">
-        <v>0</v>
-      </c>
-      <c r="Y10" s="80"/>
+      <c r="P10" s="70"/>
+      <c r="Q10" s="77"/>
+      <c r="R10" s="77"/>
+      <c r="S10" s="71">
+        <v>0</v>
+      </c>
+      <c r="T10" s="71">
+        <v>0</v>
+      </c>
+      <c r="U10" s="74">
+        <v>0</v>
+      </c>
+      <c r="V10" s="74">
+        <v>0</v>
+      </c>
+      <c r="W10" s="74">
+        <v>0</v>
+      </c>
+      <c r="X10" s="78"/>
+      <c r="Y10" s="77"/>
       <c r="Z10" s="79"/>
-      <c r="AA10" s="81"/>
-      <c r="AB10" s="82"/>
-      <c r="AC10" s="82"/>
-      <c r="AD10" s="79"/>
-      <c r="AE10" s="79"/>
-    </row>
-    <row r="11" spans="1:31">
-      <c r="A11" s="83"/>
-      <c r="B11" s="71"/>
-      <c r="C11" s="72"/>
-      <c r="D11" s="72"/>
-      <c r="E11" s="73"/>
-      <c r="F11" s="74"/>
-      <c r="G11" s="75"/>
-      <c r="H11" s="75"/>
-      <c r="I11" s="76"/>
-      <c r="J11" s="76"/>
-      <c r="K11" s="75"/>
-      <c r="L11" s="76"/>
-      <c r="M11" s="76"/>
-      <c r="N11" s="77"/>
+      <c r="AA10" s="80"/>
+      <c r="AB10" s="80"/>
+      <c r="AC10" s="77"/>
+      <c r="AD10" s="77"/>
+    </row>
+    <row r="11" spans="1:30">
+      <c r="A11" s="81"/>
+      <c r="B11" s="70"/>
+      <c r="C11" s="71"/>
+      <c r="D11" s="71"/>
+      <c r="E11" s="72"/>
+      <c r="F11" s="73"/>
+      <c r="G11" s="73"/>
+      <c r="H11" s="74"/>
+      <c r="I11" s="74"/>
+      <c r="J11" s="73"/>
+      <c r="K11" s="74"/>
+      <c r="L11" s="74"/>
+      <c r="M11" s="75"/>
+      <c r="N11" s="74"/>
       <c r="O11" s="76"/>
-      <c r="P11" s="78"/>
-      <c r="Q11" s="71"/>
-      <c r="R11" s="79"/>
-      <c r="S11" s="79"/>
-      <c r="T11" s="72"/>
-      <c r="U11" s="72"/>
-      <c r="V11" s="76"/>
-      <c r="W11" s="76"/>
-      <c r="X11" s="76"/>
-      <c r="Y11" s="80"/>
+      <c r="P11" s="70"/>
+      <c r="Q11" s="77"/>
+      <c r="R11" s="77"/>
+      <c r="S11" s="71"/>
+      <c r="T11" s="71"/>
+      <c r="U11" s="74"/>
+      <c r="V11" s="74"/>
+      <c r="W11" s="74"/>
+      <c r="X11" s="78"/>
+      <c r="Y11" s="77"/>
       <c r="Z11" s="79"/>
-      <c r="AA11" s="81"/>
-      <c r="AB11" s="82"/>
-      <c r="AC11" s="82"/>
-      <c r="AD11" s="79"/>
-      <c r="AE11" s="79"/>
-    </row>
-    <row r="12" spans="1:31">
-      <c r="A12" s="83"/>
-      <c r="B12" s="71"/>
-      <c r="C12" s="72"/>
-      <c r="D12" s="72"/>
-      <c r="E12" s="73"/>
-      <c r="F12" s="74"/>
-      <c r="G12" s="75"/>
-      <c r="H12" s="75"/>
-      <c r="I12" s="76"/>
-      <c r="J12" s="76"/>
-      <c r="K12" s="75"/>
-      <c r="L12" s="76"/>
-      <c r="M12" s="76"/>
-      <c r="N12" s="77"/>
+      <c r="AA11" s="80"/>
+      <c r="AB11" s="80"/>
+      <c r="AC11" s="77"/>
+      <c r="AD11" s="77"/>
+    </row>
+    <row r="12" spans="1:30">
+      <c r="A12" s="81"/>
+      <c r="B12" s="70"/>
+      <c r="C12" s="71"/>
+      <c r="D12" s="71"/>
+      <c r="E12" s="72"/>
+      <c r="F12" s="73"/>
+      <c r="G12" s="73"/>
+      <c r="H12" s="74"/>
+      <c r="I12" s="74"/>
+      <c r="J12" s="73"/>
+      <c r="K12" s="74"/>
+      <c r="L12" s="74"/>
+      <c r="M12" s="75"/>
+      <c r="N12" s="74"/>
       <c r="O12" s="76"/>
-      <c r="P12" s="78"/>
-      <c r="Q12" s="71"/>
-      <c r="R12" s="79"/>
-      <c r="S12" s="79"/>
-      <c r="T12" s="72"/>
-      <c r="U12" s="72"/>
-      <c r="V12" s="76"/>
-      <c r="W12" s="76"/>
-      <c r="X12" s="76"/>
-      <c r="Y12" s="80"/>
+      <c r="P12" s="70"/>
+      <c r="Q12" s="77"/>
+      <c r="R12" s="77"/>
+      <c r="S12" s="71"/>
+      <c r="T12" s="71"/>
+      <c r="U12" s="74"/>
+      <c r="V12" s="74"/>
+      <c r="W12" s="74"/>
+      <c r="X12" s="78"/>
+      <c r="Y12" s="77"/>
       <c r="Z12" s="79"/>
-      <c r="AA12" s="81"/>
-      <c r="AB12" s="82"/>
-      <c r="AC12" s="82"/>
-      <c r="AD12" s="79"/>
-      <c r="AE12" s="79"/>
-    </row>
-    <row r="13" spans="1:31" ht="12.75" customHeight="1">
-      <c r="A13" s="84" t="s">
+      <c r="AA12" s="80"/>
+      <c r="AB12" s="80"/>
+      <c r="AC12" s="77"/>
+      <c r="AD12" s="77"/>
+    </row>
+    <row r="13" spans="1:30" ht="12.75" customHeight="1">
+      <c r="A13" s="82" t="s">
         <v>69</v>
       </c>
-      <c r="B13" s="85"/>
-      <c r="C13" s="86">
+      <c r="B13" s="83"/>
+      <c r="C13" s="84">
         <f>SUM(C10:C12)</f>
         <v>0</v>
       </c>
-      <c r="D13" s="86">
+      <c r="D13" s="84">
         <f>SUM(D10:D12)</f>
         <v>0</v>
       </c>
-      <c r="E13" s="87"/>
-      <c r="F13" s="88"/>
-      <c r="G13" s="89">
-        <f t="shared" ref="G13:H13" si="0">SUM(G10:G12)</f>
-        <v>0</v>
-      </c>
-      <c r="H13" s="89">
+      <c r="E13" s="85"/>
+      <c r="F13" s="86">
+        <f t="shared" ref="F13:G13" si="0">SUM(F10:F12)</f>
+        <v>0</v>
+      </c>
+      <c r="G13" s="86">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I13" s="86"/>
-      <c r="J13" s="86"/>
-      <c r="K13" s="89">
-        <f>SUM(K10:K12)</f>
-        <v>0</v>
-      </c>
-      <c r="L13" s="86"/>
-      <c r="M13" s="86"/>
-      <c r="N13" s="90">
-        <f>SUM(N10:N12)</f>
-        <v>0</v>
-      </c>
-      <c r="O13" s="86"/>
-      <c r="P13" s="91"/>
-      <c r="Q13" s="92"/>
-      <c r="R13" s="92"/>
-      <c r="S13" s="92"/>
-      <c r="T13" s="86">
-        <f t="shared" ref="T13:X13" si="1">SUM(T10:T12)</f>
-        <v>0</v>
-      </c>
-      <c r="U13" s="86" t="e">
-        <f>V13*N13</f>
+      <c r="H13" s="84"/>
+      <c r="I13" s="84"/>
+      <c r="J13" s="86">
+        <f>SUM(J10:J12)</f>
+        <v>0</v>
+      </c>
+      <c r="K13" s="84"/>
+      <c r="L13" s="84"/>
+      <c r="M13" s="87">
+        <f>SUM(M10:M12)</f>
+        <v>0</v>
+      </c>
+      <c r="N13" s="84"/>
+      <c r="O13" s="88"/>
+      <c r="P13" s="89"/>
+      <c r="Q13" s="89"/>
+      <c r="R13" s="89"/>
+      <c r="S13" s="84">
+        <f t="shared" ref="S13:W13" si="1">SUM(S10:S12)</f>
+        <v>0</v>
+      </c>
+      <c r="T13" s="84" t="e">
+        <f>U13*M13</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="V13" s="86" t="e">
-        <f>T13/N13/12</f>
+      <c r="U13" s="84" t="e">
+        <f>S13/M13/12</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="W13" s="86" t="e">
-        <f>V13*12</f>
+      <c r="V13" s="84" t="e">
+        <f>U13*12</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="X13" s="86">
+      <c r="W13" s="84">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Y13" s="80"/>
-      <c r="Z13" s="92"/>
-      <c r="AA13" s="91"/>
-      <c r="AB13" s="93"/>
-      <c r="AC13" s="93"/>
-      <c r="AD13" s="92"/>
-      <c r="AE13" s="92"/>
-    </row>
-    <row r="14" spans="1:31" ht="9" customHeight="1">
-      <c r="A14" s="94" t="s">
-        <v>23</v>
-      </c>
-      <c r="B14" s="94" t="s">
-        <v>23</v>
-      </c>
-      <c r="C14" s="94" t="s">
-        <v>23</v>
-      </c>
-      <c r="D14" s="94" t="s">
-        <v>23</v>
-      </c>
-      <c r="E14" s="94" t="s">
-        <v>23</v>
-      </c>
-      <c r="F14" s="94"/>
-      <c r="G14" s="94" t="s">
-        <v>23</v>
-      </c>
-      <c r="H14" s="94" t="s">
-        <v>23</v>
-      </c>
-      <c r="I14" s="94" t="s">
-        <v>23</v>
-      </c>
-      <c r="J14" s="94" t="s">
-        <v>23</v>
-      </c>
-      <c r="K14" s="94" t="s">
-        <v>23</v>
-      </c>
-      <c r="L14" s="94" t="s">
-        <v>23</v>
-      </c>
-      <c r="M14" s="94" t="s">
-        <v>23</v>
-      </c>
-      <c r="N14" s="94" t="s">
-        <v>23</v>
-      </c>
-      <c r="O14" s="94" t="s">
-        <v>23</v>
-      </c>
-      <c r="P14" s="94" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q14" s="94" t="s">
-        <v>23</v>
-      </c>
-      <c r="R14" s="94" t="s">
-        <v>23</v>
-      </c>
-      <c r="S14" s="94" t="s">
-        <v>23</v>
-      </c>
-      <c r="T14" s="94" t="s">
-        <v>23</v>
-      </c>
-      <c r="U14" s="94" t="s">
-        <v>23</v>
-      </c>
-      <c r="V14" s="94" t="s">
-        <v>23</v>
-      </c>
-      <c r="W14" s="94" t="s">
-        <v>23</v>
-      </c>
-      <c r="X14" s="94" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y14" s="94" t="s">
-        <v>23</v>
-      </c>
-      <c r="Z14" s="94" t="s">
-        <v>23</v>
-      </c>
-      <c r="AA14" s="94" t="s">
-        <v>23</v>
-      </c>
-      <c r="AB14" s="94" t="s">
-        <v>23</v>
-      </c>
-      <c r="AC14" s="94" t="s">
-        <v>23</v>
-      </c>
-      <c r="AD14" s="94" t="s">
-        <v>23</v>
-      </c>
-      <c r="AE14" s="94" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="15" spans="1:31">
-      <c r="N15" s="95"/>
-      <c r="O15" s="96"/>
+      <c r="X13" s="78"/>
+      <c r="Y13" s="89"/>
+      <c r="Z13" s="88"/>
+      <c r="AA13" s="90"/>
+      <c r="AB13" s="90"/>
+      <c r="AC13" s="89"/>
+      <c r="AD13" s="89"/>
+    </row>
+    <row r="14" spans="1:30" ht="9" customHeight="1">
+      <c r="A14" s="91" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="91" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="91" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" s="91" t="s">
+        <v>23</v>
+      </c>
+      <c r="E14" s="91" t="s">
+        <v>23</v>
+      </c>
+      <c r="F14" s="91" t="s">
+        <v>23</v>
+      </c>
+      <c r="G14" s="91" t="s">
+        <v>23</v>
+      </c>
+      <c r="H14" s="91" t="s">
+        <v>23</v>
+      </c>
+      <c r="I14" s="91" t="s">
+        <v>23</v>
+      </c>
+      <c r="J14" s="91" t="s">
+        <v>23</v>
+      </c>
+      <c r="K14" s="91" t="s">
+        <v>23</v>
+      </c>
+      <c r="L14" s="91" t="s">
+        <v>23</v>
+      </c>
+      <c r="M14" s="91" t="s">
+        <v>23</v>
+      </c>
+      <c r="N14" s="91" t="s">
+        <v>23</v>
+      </c>
+      <c r="O14" s="91" t="s">
+        <v>23</v>
+      </c>
+      <c r="P14" s="91" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q14" s="91" t="s">
+        <v>23</v>
+      </c>
+      <c r="R14" s="91" t="s">
+        <v>23</v>
+      </c>
+      <c r="S14" s="91" t="s">
+        <v>23</v>
+      </c>
+      <c r="T14" s="91" t="s">
+        <v>23</v>
+      </c>
+      <c r="U14" s="91" t="s">
+        <v>23</v>
+      </c>
+      <c r="V14" s="91" t="s">
+        <v>23</v>
+      </c>
+      <c r="W14" s="91" t="s">
+        <v>23</v>
+      </c>
+      <c r="X14" s="91" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y14" s="91" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z14" s="91" t="s">
+        <v>23</v>
+      </c>
+      <c r="AA14" s="91" t="s">
+        <v>23</v>
+      </c>
+      <c r="AB14" s="91" t="s">
+        <v>23</v>
+      </c>
+      <c r="AC14" s="91" t="s">
+        <v>23</v>
+      </c>
+      <c r="AD14" s="91" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:30">
+      <c r="M15" s="92"/>
+      <c r="N15" s="93"/>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="I6:J6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4708,6 +3733,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4724,242 +3750,242 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="22.5" customHeight="1">
-      <c r="A1" s="97" t="s">
+      <c r="A1" s="94" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="142" t="s">
+      <c r="B1" s="136" t="s">
         <v>71</v>
       </c>
-      <c r="C1" s="142"/>
-      <c r="D1" s="142"/>
-      <c r="E1" s="142"/>
-      <c r="F1" s="142"/>
-      <c r="G1" s="142"/>
-      <c r="H1" s="98"/>
+      <c r="C1" s="136"/>
+      <c r="D1" s="136"/>
+      <c r="E1" s="136"/>
+      <c r="F1" s="136"/>
+      <c r="G1" s="136"/>
+      <c r="H1" s="95"/>
     </row>
     <row r="2" spans="1:8" ht="22.5" customHeight="1">
-      <c r="A2" s="99" t="s">
+      <c r="A2" s="96" t="s">
         <v>72</v>
       </c>
-      <c r="B2" s="143" t="s">
+      <c r="B2" s="137" t="s">
         <v>73</v>
       </c>
-      <c r="C2" s="143"/>
-      <c r="D2" s="143"/>
-      <c r="E2" s="143" t="s">
+      <c r="C2" s="137"/>
+      <c r="D2" s="137"/>
+      <c r="E2" s="137" t="s">
         <v>74</v>
       </c>
-      <c r="F2" s="143"/>
-      <c r="G2" s="143"/>
-      <c r="H2" s="100"/>
+      <c r="F2" s="137"/>
+      <c r="G2" s="137"/>
+      <c r="H2" s="97"/>
     </row>
     <row r="3" spans="1:8" ht="22.5" customHeight="1">
-      <c r="A3" s="101">
+      <c r="A3" s="98">
         <f>'[1]MTL Broker - 3RD'!A3</f>
         <v>41912</v>
       </c>
-      <c r="B3" s="102" t="s">
+      <c r="B3" s="99" t="s">
         <v>75</v>
       </c>
-      <c r="C3" s="102" t="s">
+      <c r="C3" s="99" t="s">
         <v>76</v>
       </c>
-      <c r="D3" s="102" t="s">
+      <c r="D3" s="99" t="s">
         <v>77</v>
       </c>
-      <c r="E3" s="102" t="s">
+      <c r="E3" s="99" t="s">
         <v>75</v>
       </c>
-      <c r="F3" s="102" t="s">
+      <c r="F3" s="99" t="s">
         <v>76</v>
       </c>
-      <c r="G3" s="102" t="s">
+      <c r="G3" s="99" t="s">
         <v>77</v>
       </c>
-      <c r="H3" s="100"/>
+      <c r="H3" s="97"/>
     </row>
     <row r="4" spans="1:8" ht="22.5" customHeight="1">
-      <c r="A4" s="102" t="s">
+      <c r="A4" s="99" t="s">
         <v>78</v>
       </c>
-      <c r="B4" s="103">
+      <c r="B4" s="100">
         <v>49</v>
       </c>
-      <c r="C4" s="103">
+      <c r="C4" s="100">
         <v>40</v>
       </c>
-      <c r="D4" s="103">
+      <c r="D4" s="100">
         <v>274</v>
       </c>
-      <c r="E4" s="104">
-        <v>0</v>
-      </c>
-      <c r="F4" s="104">
-        <v>0</v>
-      </c>
-      <c r="G4" s="104">
-        <v>0</v>
-      </c>
-      <c r="H4" s="105">
+      <c r="E4" s="101">
+        <v>0</v>
+      </c>
+      <c r="F4" s="101">
+        <v>0</v>
+      </c>
+      <c r="G4" s="101">
+        <v>0</v>
+      </c>
+      <c r="H4" s="102">
         <f>SUM(B4:G4)</f>
         <v>363</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="22.5" customHeight="1">
-      <c r="A5" s="102" t="s">
+      <c r="A5" s="99" t="s">
         <v>44</v>
       </c>
-      <c r="B5" s="103">
+      <c r="B5" s="100">
         <v>354228</v>
       </c>
-      <c r="C5" s="103">
+      <c r="C5" s="100">
         <v>344450</v>
       </c>
-      <c r="D5" s="103">
+      <c r="D5" s="100">
         <v>2736558</v>
       </c>
-      <c r="E5" s="103">
-        <v>0</v>
-      </c>
-      <c r="F5" s="103">
-        <v>0</v>
-      </c>
-      <c r="G5" s="103">
-        <v>0</v>
-      </c>
-      <c r="H5" s="106">
+      <c r="E5" s="100">
+        <v>0</v>
+      </c>
+      <c r="F5" s="100">
+        <v>0</v>
+      </c>
+      <c r="G5" s="100">
+        <v>0</v>
+      </c>
+      <c r="H5" s="103">
         <f>SUM(B5:G5)</f>
         <v>3435236</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="22.5" customHeight="1">
-      <c r="A6" s="102" t="s">
+      <c r="A6" s="99" t="s">
         <v>46</v>
       </c>
-      <c r="B6" s="103">
+      <c r="B6" s="100">
         <f t="shared" ref="B6:G6" si="0">IF(B5=0,0,B5/12/B4)</f>
         <v>602.42857142857144</v>
       </c>
-      <c r="C6" s="103">
+      <c r="C6" s="100">
         <f t="shared" si="0"/>
         <v>717.60416666666674</v>
       </c>
-      <c r="D6" s="103">
+      <c r="D6" s="100">
         <f t="shared" si="0"/>
         <v>832.28649635036493</v>
       </c>
-      <c r="E6" s="103">
+      <c r="E6" s="100">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F6" s="103">
+      <c r="F6" s="100">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G6" s="103">
+      <c r="G6" s="100">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H6" s="106">
+      <c r="H6" s="103">
         <f>H5/12/H4</f>
         <v>788.62167125803489</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="22.5" customHeight="1">
-      <c r="A7" s="144" t="s">
+      <c r="A7" s="138" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="145"/>
-      <c r="C7" s="145"/>
-      <c r="D7" s="145"/>
-      <c r="E7" s="145"/>
-      <c r="F7" s="145"/>
-      <c r="G7" s="146"/>
-      <c r="H7" s="106"/>
+      <c r="B7" s="139"/>
+      <c r="C7" s="139"/>
+      <c r="D7" s="139"/>
+      <c r="E7" s="139"/>
+      <c r="F7" s="139"/>
+      <c r="G7" s="140"/>
+      <c r="H7" s="103"/>
     </row>
     <row r="8" spans="1:8" ht="22.5" customHeight="1">
-      <c r="A8" s="107" t="s">
+      <c r="A8" s="104" t="s">
         <v>78</v>
       </c>
-      <c r="B8" s="104">
+      <c r="B8" s="101">
         <v>345</v>
       </c>
-      <c r="C8" s="104">
+      <c r="C8" s="101">
         <v>332</v>
       </c>
-      <c r="D8" s="104">
+      <c r="D8" s="101">
         <v>2056</v>
       </c>
-      <c r="E8" s="104">
+      <c r="E8" s="101">
         <v>1</v>
       </c>
-      <c r="F8" s="104">
+      <c r="F8" s="101">
         <v>2</v>
       </c>
-      <c r="G8" s="104">
+      <c r="G8" s="101">
         <v>5</v>
       </c>
-      <c r="H8" s="105">
+      <c r="H8" s="102">
         <f>SUM(B8:G8)</f>
         <v>2741</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="22.5" customHeight="1">
-      <c r="A9" s="107" t="s">
+      <c r="A9" s="104" t="s">
         <v>44</v>
       </c>
-      <c r="B9" s="104">
+      <c r="B9" s="101">
         <v>2388632</v>
       </c>
-      <c r="C9" s="104">
+      <c r="C9" s="101">
         <v>2901090</v>
       </c>
-      <c r="D9" s="104">
+      <c r="D9" s="101">
         <v>20093654</v>
       </c>
-      <c r="E9" s="104">
+      <c r="E9" s="101">
         <v>15912</v>
       </c>
-      <c r="F9" s="104">
+      <c r="F9" s="101">
         <v>34044</v>
       </c>
-      <c r="G9" s="104">
+      <c r="G9" s="101">
         <v>99792</v>
       </c>
-      <c r="H9" s="106">
+      <c r="H9" s="103">
         <f>SUM(B9:G9)</f>
         <v>25533124</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="22.5" customHeight="1">
-      <c r="A10" s="107" t="s">
+      <c r="A10" s="104" t="s">
         <v>46</v>
       </c>
-      <c r="B10" s="103">
+      <c r="B10" s="100">
         <f t="shared" ref="B10:G10" si="1">IF(B9=0,0,B9/12/B8)</f>
         <v>576.96425120772949</v>
       </c>
-      <c r="C10" s="103">
+      <c r="C10" s="100">
         <f t="shared" si="1"/>
         <v>728.18524096385545</v>
       </c>
-      <c r="D10" s="103">
+      <c r="D10" s="100">
         <f t="shared" si="1"/>
         <v>814.43150129701689</v>
       </c>
-      <c r="E10" s="103">
+      <c r="E10" s="100">
         <f t="shared" si="1"/>
         <v>1326</v>
       </c>
-      <c r="F10" s="103">
+      <c r="F10" s="100">
         <f t="shared" si="1"/>
         <v>1418.5</v>
       </c>
-      <c r="G10" s="103">
+      <c r="G10" s="100">
         <f t="shared" si="1"/>
         <v>1663.2</v>
       </c>
-      <c r="H10" s="106">
+      <c r="H10" s="103">
         <f>H9/12/H8</f>
         <v>776.27155539340879</v>
       </c>
@@ -4973,4 +3999,135 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="35.7109375" customWidth="1"/>
+    <col min="2" max="2" width="32.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="141" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="141" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A2" s="142" t="s">
+        <v>79</v>
+      </c>
+      <c r="B2" s="143" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A3" s="142" t="s">
+        <v>81</v>
+      </c>
+      <c r="B3" s="143" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A4" s="142" t="s">
+        <v>83</v>
+      </c>
+      <c r="B4" s="143" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A5" s="142" t="s">
+        <v>85</v>
+      </c>
+      <c r="B5" s="144" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A6" s="142" t="s">
+        <v>87</v>
+      </c>
+      <c r="B6" s="145" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A7" s="142" t="s">
+        <v>89</v>
+      </c>
+      <c r="B7" s="145" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A8" s="142" t="s">
+        <v>91</v>
+      </c>
+      <c r="B8" s="143" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A9" s="142" t="s">
+        <v>93</v>
+      </c>
+      <c r="B9" s="146" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A10" s="142" t="s">
+        <v>95</v>
+      </c>
+      <c r="B10" s="143" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A11" s="142" t="s">
+        <v>97</v>
+      </c>
+      <c r="B11" s="144" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A12" s="142" t="s">
+        <v>99</v>
+      </c>
+      <c r="B12" s="143" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A13" s="142" t="s">
+        <v>101</v>
+      </c>
+      <c r="B13" s="145" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A14" s="142" t="s">
+        <v>103</v>
+      </c>
+      <c r="B14" s="143" t="s">
+        <v>104</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>